<commit_message>
Glycan work and cleaning
</commit_message>
<xml_diff>
--- a/Python_output_files/Tables/differential_glycomics_cohort.xlsx
+++ b/Python_output_files/Tables/differential_glycomics_cohort.xlsx
@@ -487,25 +487,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.446454418833357</v>
+        <v>2.442886703275678</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.4867804366063924</v>
+        <v>-0.4749816135202121</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0006602311561742895</v>
+        <v>0.0006234348210585188</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03096294867952351</v>
+        <v>0.03862918826517468</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8536406916510157</v>
+        <v>0.5970596995326609</v>
       </c>
       <c r="H2" t="n">
-        <v>-2.19916358923596</v>
+        <v>-2.267405647329488</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -518,25 +518,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.006225203827561906</v>
+        <v>0.006216564666903516</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.4796227384275196</v>
+        <v>-0.4593613383824571</v>
       </c>
       <c r="D3" t="n">
-        <v>0.000711791923667207</v>
+        <v>0.0008680716464084195</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03096294867952351</v>
+        <v>0.03862918826517468</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8421589240717978</v>
+        <v>0.7661233146213616</v>
       </c>
       <c r="H3" t="n">
-        <v>-2.157784362321063</v>
+        <v>-2.10806841701938</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -545,29 +545,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Man</t>
+          <t>Terminal_Fuc(a1-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.04362323645437521</v>
+        <v>10.56108234393164</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.6677745502136962</v>
+        <v>-0.5440540002858034</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001232796283974127</v>
+        <v>0.002144464679305054</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03292066259062938</v>
+        <v>0.04305487782726693</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5556987528519068</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H4" t="n">
-        <v>-2.04206580892326</v>
+        <v>-1.945368484929183</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -576,29 +576,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)Gal(b1-?)</t>
+          <t>Terminal_Fuc(a1-2)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.5762389829412</v>
+        <v>12.03159652417705</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.5519665244939072</v>
+        <v>-0.550173591275029</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001985885397541725</v>
+        <v>0.002719003612169723</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03292066259062938</v>
+        <v>0.04305487782726693</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.2740857702405718</v>
       </c>
       <c r="H5" t="n">
-        <v>-1.971605959635389</v>
+        <v>-1.909852209712644</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -611,25 +611,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.277174617813642</v>
+        <v>2.273099227481542</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.432198565678906</v>
+        <v>-0.4174851508010358</v>
       </c>
       <c r="D6" t="n">
-        <v>0.002265919704161518</v>
+        <v>0.002873610006807179</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03292066259062938</v>
+        <v>0.04305487782726693</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2962786121219571</v>
+        <v>0.2590594958703056</v>
       </c>
       <c r="H6" t="n">
-        <v>-2.000095028822521</v>
+        <v>-1.985469955548685</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -638,29 +638,29 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)</t>
+          <t>Terminal_Fuc(a1-?)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12.02327367805511</v>
+        <v>12.47592352123545</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.5543901729167136</v>
+        <v>-0.5483965886272362</v>
       </c>
       <c r="D7" t="n">
-        <v>0.002465922537264794</v>
+        <v>0.002902576033298894</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03292066259062938</v>
+        <v>0.04305487782726693</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2740857702405718</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.934385133953631</v>
+        <v>-1.892182729532331</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -669,29 +669,29 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)</t>
+          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Man</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12.46893219001151</v>
+        <v>0.04356442347863602</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.5520448173126091</v>
+        <v>-0.6319073538655864</v>
       </c>
       <c r="D8" t="n">
-        <v>0.002648788944073628</v>
+        <v>0.00342545819944171</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03292066259062938</v>
+        <v>0.04355225425004459</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.4495989354798668</v>
       </c>
       <c r="H8" t="n">
-        <v>-1.915448555648645</v>
+        <v>-1.796152694362217</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -700,29 +700,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)[Gal(a1-3)]Gal</t>
+          <t>Terminal_Fuc(a1-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.05544185043309365</v>
+        <v>8.337094690260317</v>
       </c>
       <c r="C9" t="n">
-        <v>1.401224919741851</v>
+        <v>-0.5670372109455233</v>
       </c>
       <c r="D9" t="n">
-        <v>0.003514472085762879</v>
+        <v>0.004383138176615814</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03821988393267131</v>
+        <v>0.04876241221485093</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4050435206247978</v>
+        <v>0.2509866995169991</v>
       </c>
       <c r="H9" t="n">
-        <v>1.896444316693413</v>
+        <v>-1.770053592940314</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
@@ -731,29 +731,29 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_Fuc(a1-2)[Gal(a1-3)]Gal</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8.348281011733089</v>
+        <v>0.05532813847712449</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.5729807882322735</v>
+        <v>1.414696378618648</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003994640555600588</v>
+        <v>0.005029803720018671</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03861485870413902</v>
+        <v>0.04973917012018464</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.3593354328337088</v>
       </c>
       <c r="H10" t="n">
-        <v>-1.797518092730751</v>
+        <v>1.806149406130935</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -762,29 +762,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)[GlcNAc(b1-6)]GalNAc</t>
+          <t>Terminal_HexNAc(?1-?)GlcNAc(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2421747528941239</v>
+        <v>0.09214002274701549</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.5636937288653514</v>
+        <v>-0.8160553847220235</v>
       </c>
       <c r="D11" t="n">
-        <v>0.005962304314171033</v>
+        <v>0.005697241125674827</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04859868361214673</v>
+        <v>0.05070544601850595</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5292082949514116</v>
+        <v>0.3256857630054634</v>
       </c>
       <c r="H11" t="n">
-        <v>-1.70897805164784</v>
+        <v>-1.674365875703033</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -793,29 +793,29 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_Gal(b1-3)[GlcNAc(b1-6)]GalNAc</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6.609852956311165</v>
+        <v>0.2418350215474748</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.5415276643676474</v>
+        <v>-0.5104155586520402</v>
       </c>
       <c r="D12" t="n">
-        <v>0.006345968597107113</v>
+        <v>0.007493954057019067</v>
       </c>
       <c r="E12" t="n">
-        <v>0.04859868361214673</v>
+        <v>0.05558015925622475</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.5970596995326609</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.674010368696537</v>
+        <v>-1.628214262441523</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
@@ -824,29 +824,29 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAcOS(b1-6)GalNAc</t>
+          <t>Terminal_Fuc(a1-2)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.03702819077954295</v>
+        <v>6.600218244728373</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9098308023943465</v>
+        <v>-0.5302857555520522</v>
       </c>
       <c r="D13" t="n">
-        <v>0.006703266705123686</v>
+        <v>0.007269004368296858</v>
       </c>
       <c r="E13" t="n">
-        <v>0.04859868361214673</v>
+        <v>0.05558015925622475</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0.7402342971192114</v>
+        <v>0.2509866995169991</v>
       </c>
       <c r="H13" t="n">
-        <v>1.592249741798445</v>
+        <v>-1.634083208066293</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
@@ -855,29 +855,29 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)[Fuc(a1-?)]GalNAc</t>
+          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0165613952646341</v>
+        <v>1.156451531767201</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.5417265481578197</v>
+        <v>-0.4951858006055012</v>
       </c>
       <c r="D14" t="n">
-        <v>0.009009003360315968</v>
+        <v>0.01750288359132655</v>
       </c>
       <c r="E14" t="n">
-        <v>0.04949277215063207</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4050435206247978</v>
+        <v>0.4541448710731509</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.593933498714746</v>
+        <v>-1.419880084795149</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -886,29 +886,29 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)GlcNAc(b1-?)GalNAc</t>
+          <t>Terminal_GlcNAcOS(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.09225137569640053</v>
+        <v>0.03694834607758393</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.791292412597236</v>
+        <v>0.849387478647742</v>
       </c>
       <c r="D15" t="n">
-        <v>0.009156678914179775</v>
+        <v>0.01094538992787064</v>
       </c>
       <c r="E15" t="n">
-        <v>0.04949277215063207</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.757390061970881</v>
       </c>
       <c r="H15" t="n">
-        <v>-1.557827309944916</v>
+        <v>1.466949084711049</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
@@ -917,29 +917,29 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)GalNAc</t>
+          <t>Terminal_Fuc(a1-?)Gal(?1-?)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6922407317589299</v>
+        <v>1.446584334467115</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.4596754426312732</v>
+        <v>-0.7028634365859006</v>
       </c>
       <c r="D16" t="n">
-        <v>0.009221211481922752</v>
+        <v>0.01222675806261473</v>
       </c>
       <c r="E16" t="n">
-        <v>0.04949277215063207</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.8207392877422073</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H16" t="n">
-        <v>-1.56408084025501</v>
+        <v>-1.600217105931865</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -948,29 +948,29 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)GlcNAc(b1-6)GalNAc</t>
+          <t>Terminal_Fuc(a1-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.147979939572018</v>
+        <v>1.437171270662088</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.5512351169526903</v>
+        <v>-0.7013493681036973</v>
       </c>
       <c r="D17" t="n">
-        <v>0.009458396355786537</v>
+        <v>0.01231176770613889</v>
       </c>
       <c r="E17" t="n">
-        <v>0.04949277215063207</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.5556987528519068</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H17" t="n">
-        <v>-1.596304651667978</v>
+        <v>-1.598431148031233</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
@@ -979,29 +979,29 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)GalNAc</t>
+          <t>Terminal_GlcNAc(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.158113350996088</v>
+        <v>0.8675720114709319</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.5490434727873019</v>
+        <v>-0.4587117687007218</v>
       </c>
       <c r="D18" t="n">
-        <v>0.009671001454721209</v>
+        <v>0.01552473425628297</v>
       </c>
       <c r="E18" t="n">
-        <v>0.04949277215063207</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.5556987528519068</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.591551370850137</v>
+        <v>-1.425944393129423</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
@@ -1010,29 +1010,29 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)</t>
+          <t>Terminal_GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.008709118343494</v>
+        <v>0.8811677471638477</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.4191036215321278</v>
+        <v>-0.4462355026388689</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01038658578424702</v>
+        <v>0.01558476594469633</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05020183129052724</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.676156396713796</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H19" t="n">
-        <v>-1.544593423439028</v>
+        <v>-1.416602282094755</v>
       </c>
       <c r="I19" t="n">
         <v>1</v>
@@ -1041,29 +1041,29 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(b1-6)GalNAc</t>
+          <t>Terminal_Gal(b1-3)</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.8653899404112582</v>
+        <v>1.007259911428097</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.5033840698851249</v>
+        <v>-0.4017433152752421</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01224946841168147</v>
+        <v>0.01615667045401882</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0533530863240396</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2734859319944637</v>
+        <v>0.6197386739134845</v>
       </c>
       <c r="H20" t="n">
-        <v>-1.501767594743559</v>
+        <v>-1.426752764461275</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
@@ -1072,29 +1072,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(b1-?)</t>
+          <t>Terminal_Gal(b1-?)[Fuc(a1-?)]GalNAc</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.8790049522615168</v>
+        <v>0.01653737665202215</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.4893647868687738</v>
+        <v>-0.5062046216299522</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01291180546587829</v>
+        <v>0.0165330543733158</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0533530863240396</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2962786121219571</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H21" t="n">
-        <v>-1.479747927886193</v>
+        <v>-1.428939519437039</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
@@ -1103,29 +1103,29 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.413608378235235</v>
+        <v>0.6912675488099826</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.6792889090176679</v>
+        <v>-0.4501694156813811</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01345486953945108</v>
+        <v>0.01676595821073696</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0533530863240396</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.5970596995326609</v>
       </c>
       <c r="H22" t="n">
-        <v>-1.553121619383986</v>
+        <v>-1.414019730072965</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
@@ -1134,29 +1134,29 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)Gal(?1-?)</t>
+          <t>Terminal_Gal(b1-4)GlcNAc(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.423061433251569</v>
+        <v>1.146335110011408</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.6801756426957128</v>
+        <v>-0.49740865352583</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01349158504745829</v>
+        <v>0.01734128700665536</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0533530863240396</v>
+        <v>0.07080711998309377</v>
       </c>
       <c r="F23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.4605765235170522</v>
       </c>
       <c r="H23" t="n">
-        <v>-1.552152541055091</v>
+        <v>-1.421667145945541</v>
       </c>
       <c r="I23" t="n">
         <v>1</v>
@@ -1165,29 +1165,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)</t>
+          <t>Terminal_GalNAc(a1-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2.71272881999338</v>
+        <v>0.199986308707129</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.4435476162815508</v>
+        <v>-0.6190072957307478</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02010823179704337</v>
+        <v>0.02561976721888945</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0760615724496858</v>
+        <v>0.09120637129924644</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.4050435206247978</v>
+        <v>0.2740857702405718</v>
       </c>
       <c r="H24" t="n">
-        <v>-1.387335535036028</v>
+        <v>-1.269979032091894</v>
       </c>
       <c r="I24" t="n">
         <v>1</v>
@@ -1196,29 +1196,29 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.94619445454401</v>
+        <v>0.5661542979813585</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.4710145947269044</v>
+        <v>-0.4586612909386689</v>
       </c>
       <c r="D25" t="n">
-        <v>0.02158598107053403</v>
+        <v>0.02555215285017954</v>
       </c>
       <c r="E25" t="n">
-        <v>0.07824918138068584</v>
+        <v>0.09120637129924644</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0.3517918066608662</v>
+        <v>0.448244648544068</v>
       </c>
       <c r="H25" t="n">
-        <v>-1.372888176528059</v>
+        <v>-1.312935816503308</v>
       </c>
       <c r="I25" t="n">
         <v>1</v>
@@ -1227,29 +1227,29 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-4)Gal(b1-3)GalNAc</t>
+          <t>Terminal_GalNAc(a1-3)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.5507130016182282</v>
+        <v>0.05457231974549027</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.47239288132974</v>
+        <v>-0.7199804180482897</v>
       </c>
       <c r="D26" t="n">
-        <v>0.02276492757213662</v>
+        <v>0.02510680275908036</v>
       </c>
       <c r="E26" t="n">
-        <v>0.07922194795103542</v>
+        <v>0.09120637129924644</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0.414486109107268</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H26" t="n">
-        <v>-1.344945630248882</v>
+        <v>-1.274644479936393</v>
       </c>
       <c r="I26" t="n">
         <v>1</v>
@@ -1258,29 +1258,29 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)</t>
+          <t>Terminal_Gal(b1-?)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.556897223673147</v>
+        <v>2.708406815691356</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.4616505575743357</v>
+        <v>-0.4202869375918361</v>
       </c>
       <c r="D27" t="n">
-        <v>0.02574368960847573</v>
+        <v>0.03043903994665786</v>
       </c>
       <c r="E27" t="n">
-        <v>0.08614234599759187</v>
+        <v>0.1038856732817187</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.3292112483650667</v>
+        <v>0.333625736668872</v>
       </c>
       <c r="H27" t="n">
-        <v>-1.316671941738651</v>
+        <v>-1.268705823165823</v>
       </c>
       <c r="I27" t="n">
         <v>1</v>
@@ -1289,29 +1289,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-6)GlcNAc</t>
+          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.06599609523156567</v>
+        <v>1.942981925810733</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.6756801583776491</v>
+        <v>-0.4409784501556739</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0287088633166017</v>
+        <v>0.03263618550667336</v>
       </c>
       <c r="E28" t="n">
-        <v>0.09250633735349437</v>
+        <v>0.1038856732817187</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.3135975153090783</v>
       </c>
       <c r="H28" t="n">
-        <v>-1.316454306287728</v>
+        <v>-1.251867457370228</v>
       </c>
       <c r="I28" t="n">
         <v>1</v>
@@ -1320,29 +1320,29 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Gal</t>
+          <t>Terminal_Gal(b1-4)</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.8930763116150742</v>
+        <v>1.554243513717596</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.5697260724013375</v>
+        <v>-0.4415135858381563</v>
       </c>
       <c r="D29" t="n">
-        <v>0.03400345757370864</v>
+        <v>0.03310201557992307</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1038800604247341</v>
+        <v>0.1038856732817187</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0.9289816354296266</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H29" t="n">
-        <v>-1.217064268540143</v>
+        <v>-1.242801264339413</v>
       </c>
       <c r="I29" t="n">
         <v>1</v>
@@ -1351,29 +1351,29 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)GalNAc</t>
+          <t>Terminal_Gal(?1-?)</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.02669480668870429</v>
+        <v>1.883150074224277</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.429130541567055</v>
+        <v>-0.4909959252769385</v>
       </c>
       <c r="D30" t="n">
-        <v>0.03462668680824469</v>
+        <v>0.03574597825390973</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1038800604247341</v>
+        <v>0.1038856732817187</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.5292082949514116</v>
+        <v>0.7661233146213616</v>
       </c>
       <c r="H30" t="n">
-        <v>-1.193476412236795</v>
+        <v>-1.209731793744402</v>
       </c>
       <c r="I30" t="n">
         <v>1</v>
@@ -1382,29 +1382,29 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)</t>
+          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1.883269643174301</v>
+        <v>1.84403211266834</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.4800042716445798</v>
+        <v>-0.4969909294780823</v>
       </c>
       <c r="D31" t="n">
-        <v>0.03763239789785348</v>
+        <v>0.03623184847258426</v>
       </c>
       <c r="E31" t="n">
-        <v>0.1067729340914086</v>
+        <v>0.1038856732817187</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.7813200710667018</v>
+        <v>0.7661233146213616</v>
       </c>
       <c r="H31" t="n">
-        <v>-1.193460969055666</v>
+        <v>-1.207064731172394</v>
       </c>
       <c r="I31" t="n">
         <v>1</v>
@@ -1413,29 +1413,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Gal</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1.844065517333669</v>
+        <v>0.8918373457620604</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.4862495632715431</v>
+        <v>-0.5757065749758041</v>
       </c>
       <c r="D32" t="n">
-        <v>0.03804552823946743</v>
+        <v>0.03678898531440652</v>
       </c>
       <c r="E32" t="n">
-        <v>0.1067729340914086</v>
+        <v>0.1038856732817187</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0.7813200710667018</v>
+        <v>0.7767515869384096</v>
       </c>
       <c r="H32" t="n">
-        <v>-1.191537259992172</v>
+        <v>-1.197606771831858</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -1444,29 +1444,29 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-3)Gal</t>
+          <t>Terminal_Fuc(a1-6)GlcNAc</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.2089698300111693</v>
+        <v>0.06583222709782377</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.3916616553332166</v>
+        <v>-0.6914606813851039</v>
       </c>
       <c r="D33" t="n">
-        <v>0.04520869787331172</v>
+        <v>0.03735215219117977</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1199061028253448</v>
+        <v>0.1038856732817187</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.8421589240717978</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H33" t="n">
-        <v>-1.102184233606293</v>
+        <v>-1.238958981541067</v>
       </c>
       <c r="I33" t="n">
         <v>1</v>
@@ -1475,29 +1475,29 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(a1-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_Fuc(a1-?)GalNAc</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.2002344705931141</v>
+        <v>0.02665379840781519</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.5683651520218493</v>
+        <v>-0.3861714854935747</v>
       </c>
       <c r="D34" t="n">
-        <v>0.04548162520961353</v>
+        <v>0.03918541524442865</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1199061028253448</v>
+        <v>0.1056818774773985</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.6197386739134845</v>
       </c>
       <c r="H34" t="n">
-        <v>-1.117966852352586</v>
+        <v>-1.151326992469048</v>
       </c>
       <c r="I34" t="n">
         <v>1</v>
@@ -1506,32 +1506,32 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(a1-3)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_GlcNAc(a1-4)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.05463922453026073</v>
+        <v>0.5502952179280234</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.6527185016830032</v>
+        <v>-0.4560132987548764</v>
       </c>
       <c r="D35" t="n">
-        <v>0.05345874550545804</v>
+        <v>0.04074200324754399</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1304403954364958</v>
+        <v>0.1066481849715122</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2645821994686438</v>
+        <v>0.4107312271350288</v>
       </c>
       <c r="H35" t="n">
-        <v>-1.0751176221369</v>
+        <v>-1.184331867002698</v>
       </c>
       <c r="I35" t="n">
-        <v>0.9523706226862587</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1541,338 +1541,338 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.9073659692642193</v>
+        <v>0.9086303434276433</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.4003307316166715</v>
+        <v>-0.4205028215009881</v>
       </c>
       <c r="D36" t="n">
-        <v>0.05394154476698002</v>
+        <v>0.04406796183964379</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1304403954364958</v>
+        <v>0.1089457945480083</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0.5556987528519068</v>
+        <v>0.5970596995326609</v>
       </c>
       <c r="H36" t="n">
-        <v>-1.094519507174449</v>
+        <v>-1.155018021881777</v>
       </c>
       <c r="I36" t="n">
-        <v>0.9523706226862587</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_Fuc(a1-2)Gal(b1-3)GlcNAc</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.5669784767649626</v>
+        <v>0.2251156142712599</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.4155519524233617</v>
+        <v>-0.6049764010149188</v>
       </c>
       <c r="D37" t="n">
-        <v>0.05535785038616699</v>
+        <v>0.04303827946730408</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1304403954364958</v>
+        <v>0.1089457945480083</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0.3161976169782357</v>
+        <v>0.4605765235170522</v>
       </c>
       <c r="H37" t="n">
-        <v>-1.093503820412545</v>
+        <v>-1.123057221132168</v>
       </c>
       <c r="I37" t="n">
-        <v>0.9523706226862587</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)Gal(b1-3)GlcNAc</t>
+          <t>Terminal_GalNAc(b1-4)GlcNAc(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.2247216514528098</v>
+        <v>0.8301788165562858</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.5916474330605426</v>
+        <v>-0.4240113260839538</v>
       </c>
       <c r="D38" t="n">
-        <v>0.05547465093276257</v>
+        <v>0.05248302546582505</v>
       </c>
       <c r="E38" t="n">
-        <v>0.1304403954364958</v>
+        <v>0.1239895812095295</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>0.3940177435861071</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H38" t="n">
-        <v>-1.056515622388098</v>
+        <v>-1.062795789447656</v>
       </c>
       <c r="I38" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Terminal_GalOS(b1-3)GalNAc</t>
+          <t>Terminal_GalNAc(b1-4)</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.003335459167239692</v>
+        <v>0.8713224139862197</v>
       </c>
       <c r="C39" t="n">
-        <v>1.21609806351609</v>
+        <v>-0.4070858502378911</v>
       </c>
       <c r="D39" t="n">
-        <v>0.06164526858288135</v>
+        <v>0.05293937175238337</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1344940413797699</v>
+        <v>0.1239895812095295</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5226702430025253</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H39" t="n">
-        <v>1.06321140776903</v>
+        <v>-1.05991988439111</v>
       </c>
       <c r="I39" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)[HexNAc(?1-?)]GalNAc</t>
+          <t>Terminal_GalNAc(a1-3)Gal(b1-3)GlcNAc</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.007539255451344048</v>
+        <v>0.1454139889616387</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.3823666358301434</v>
+        <v>-0.567627883886856</v>
       </c>
       <c r="D40" t="n">
-        <v>0.06224633671694028</v>
+        <v>0.05620350509781328</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1344940413797699</v>
+        <v>0.1282592808642405</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0.552630143865133</v>
+        <v>0.5757461592689368</v>
       </c>
       <c r="H40" t="n">
-        <v>-1.019171560283268</v>
+        <v>-1.044044156052434</v>
       </c>
       <c r="I40" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)[GlcNAcOS(b1-6)]GalNAc</t>
+          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.02120432287162431</v>
+        <v>0.3129144726113906</v>
       </c>
       <c r="C41" t="n">
-        <v>0.7518324678103663</v>
+        <v>-0.474654655742047</v>
       </c>
       <c r="D41" t="n">
-        <v>0.06423944732983541</v>
+        <v>0.05889695017158856</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1344940413797699</v>
+        <v>0.1283981420674561</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.5313738697253738</v>
+        <v>0.5729731502606171</v>
       </c>
       <c r="H41" t="n">
-        <v>1.023774512848286</v>
+        <v>-1.039986450119395</v>
       </c>
       <c r="I41" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_Fuc(a1-?)[HexNAc(?1-?)]GalNAc</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.02090216834809419</v>
+        <v>0.007528206242541072</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9779633308351462</v>
+        <v>-0.3834384123510346</v>
       </c>
       <c r="D42" t="n">
-        <v>0.06630864291745839</v>
+        <v>0.05914970589624385</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1344940413797699</v>
+        <v>0.1283981420674561</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0.7402342971192114</v>
+        <v>0.4495989354798668</v>
       </c>
       <c r="H42" t="n">
-        <v>1.00034276862437</v>
+        <v>-1.034997883897619</v>
       </c>
       <c r="I42" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_GalNAc(b1-4)GlcNAc(b1-6)</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.3139597660140334</v>
+        <v>0.7759177903440656</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.464761395821176</v>
+        <v>-0.3970334560970405</v>
       </c>
       <c r="D43" t="n">
-        <v>0.06645166717107887</v>
+        <v>0.06444656786641872</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1344940413797699</v>
+        <v>0.1363090268896675</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.4900435232578885</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H43" t="n">
-        <v>-1.008217741781316</v>
+        <v>-1.00772512314662</v>
       </c>
       <c r="I43" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(b1-4)GlcNAc(b1-6)GalNAc</t>
+          <t>Terminal_HexNAc(?1-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.8318090884613162</v>
+        <v>1.079637275787552</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.3914051099301696</v>
+        <v>-0.4244743563187239</v>
       </c>
       <c r="D44" t="n">
-        <v>0.06743020484226242</v>
+        <v>0.06585717029500787</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1344940413797699</v>
+        <v>0.1363090268896675</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>0.2962786121219571</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.9951075365696253</v>
+        <v>-1.035866479009545</v>
       </c>
       <c r="I44" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(b1-4)</t>
+          <t>Terminal_GalOS(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.8730156472107304</v>
+        <v>0.003324171047890064</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.3759513073331036</v>
+        <v>1.264667839144539</v>
       </c>
       <c r="D45" t="n">
-        <v>0.06801997495068822</v>
+        <v>0.06830490075580394</v>
       </c>
       <c r="E45" t="n">
-        <v>0.1344940413797699</v>
+        <v>0.1381621856196943</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0.3094825279827125</v>
+        <v>0.448244648544068</v>
       </c>
       <c r="H45" t="n">
-        <v>-0.9920747610550009</v>
+        <v>1.036449896955615</v>
       </c>
       <c r="I45" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(a1-3)Gal(b1-3)GlcNAc</t>
+          <t>Terminal_HexNAc(?1-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.1455952460628533</v>
+        <v>0.02085292053620985</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.531031955365644</v>
+        <v>0.9760369401249167</v>
       </c>
       <c r="D46" t="n">
-        <v>0.07914576278061333</v>
+        <v>0.07004074772025404</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1530151413758525</v>
+        <v>0.138525034380058</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.5292082949514116</v>
+        <v>0.7661233146213616</v>
       </c>
       <c r="H46" t="n">
-        <v>-0.9506353600222148</v>
+        <v>0.9838143059454955</v>
       </c>
       <c r="I46" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="47">
@@ -1882,59 +1882,59 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.2654387186062059</v>
+        <v>0.2648700110660739</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.4109238982926362</v>
+        <v>-0.4125899366890855</v>
       </c>
       <c r="D47" t="n">
-        <v>0.08195104181110491</v>
+        <v>0.07230888794322156</v>
       </c>
       <c r="E47" t="n">
-        <v>0.15443620907588</v>
+        <v>0.1399019788466678</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0.2967971322525303</v>
+        <v>0.4107312271350288</v>
       </c>
       <c r="H47" t="n">
-        <v>-0.963137289653502</v>
+        <v>-0.9962657751080611</v>
       </c>
       <c r="I47" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(b1-4)GlcNAc(b1-6)</t>
+          <t>Terminal_Neu5Ac(a2-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.7770628372259267</v>
+        <v>0.4710288080281532</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.36624907525254</v>
+        <v>-0.6472818721446392</v>
       </c>
       <c r="D48" t="n">
-        <v>0.08343105547777423</v>
+        <v>0.0742181143047662</v>
       </c>
       <c r="E48" t="n">
-        <v>0.15443620907588</v>
+        <v>0.1405406845345573</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0.3161976169782357</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.9359298750304331</v>
+        <v>-1.009937781467253</v>
       </c>
       <c r="I48" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="49">
@@ -1944,307 +1944,307 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.2592135147786441</v>
+        <v>0.2586534463991704</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.4098329545207675</v>
+        <v>-0.4117541627323638</v>
       </c>
       <c r="D49" t="n">
-        <v>0.08658876392599588</v>
+        <v>0.07637598043624158</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1569421346158675</v>
+        <v>0.1416137970588646</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0.2967971322525303</v>
+        <v>0.4107312271350288</v>
       </c>
       <c r="H49" t="n">
-        <v>-0.946625401347654</v>
+        <v>-0.980051856886517</v>
       </c>
       <c r="I49" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)Gal(b1-?)</t>
+          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-3)Gal</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1.081254791959911</v>
+        <v>0.2086725526394138</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.3970085865679565</v>
+        <v>-0.3325059686154619</v>
       </c>
       <c r="D50" t="n">
-        <v>0.09639319417127157</v>
+        <v>0.07931182750874825</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1711470998551148</v>
+        <v>0.1440561764954815</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.7589117343558239</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.9231844847072096</v>
+        <v>-0.9490927694472824</v>
       </c>
       <c r="I50" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_HexNAc(?1-?)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.4540485608111793</v>
+        <v>1.451225659579324</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.6487098238776521</v>
+        <v>-0.3838800928569368</v>
       </c>
       <c r="D51" t="n">
-        <v>0.103418216729373</v>
+        <v>0.0891266160013853</v>
       </c>
       <c r="E51" t="n">
-        <v>0.179947697109109</v>
+        <v>0.1586453764824658</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H51" t="n">
-        <v>-0.9095038669611073</v>
+        <v>-0.9471243332008766</v>
       </c>
       <c r="I51" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Terminal_Gal(a1-3)Gal(b1-3)GalNAc</t>
+          <t>Terminal_Gal(b1-3)[GlcNAcOS(b1-6)]GalNAc</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.0796845149374677</v>
+        <v>0.02116028112185416</v>
       </c>
       <c r="C52" t="n">
-        <v>0.5729246569566198</v>
+        <v>0.6438126640783971</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1128369928603011</v>
+        <v>0.1098330373597501</v>
       </c>
       <c r="E52" t="n">
-        <v>0.1924866348793372</v>
+        <v>0.1916694181376032</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>0.3292112483650667</v>
+        <v>0.4605765235170522</v>
       </c>
       <c r="H52" t="n">
-        <v>0.8886021664402604</v>
+        <v>0.867267487605377</v>
       </c>
       <c r="I52" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)</t>
+          <t>Terminal_Gal(a1-3)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1.453411664201522</v>
+        <v>0.07953519695788935</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.3476688662202267</v>
+        <v>0.5834697543297036</v>
       </c>
       <c r="D53" t="n">
-        <v>0.130404953250943</v>
+        <v>0.1222391668767844</v>
       </c>
       <c r="E53" t="n">
-        <v>0.2181775179390777</v>
+        <v>0.2092170356160349</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.333625736668872</v>
       </c>
       <c r="H53" t="n">
-        <v>-0.8297926138417195</v>
+        <v>0.8638675617174355</v>
       </c>
       <c r="I53" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)HexNAc(?1-?)GlcNAc</t>
+          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.1047621667626144</v>
+        <v>0.5134829778061938</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.495191533179399</v>
+        <v>-0.3958864098149331</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1371120291437071</v>
+        <v>0.139409141652773</v>
       </c>
       <c r="E54" t="n">
-        <v>0.2250706893491041</v>
+        <v>0.2341021435301283</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>0.403654669828124</v>
+        <v>0.2385838867876085</v>
       </c>
       <c r="H54" t="n">
-        <v>-0.8380553171370377</v>
+        <v>-0.8058365932791133</v>
       </c>
       <c r="I54" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-3)Man(b1-4)GlcNAc</t>
+          <t>Terminal_HexNAc(b1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.07510403696942346</v>
+        <v>0.406577400136074</v>
       </c>
       <c r="C55" t="n">
-        <v>0.5346507183953457</v>
+        <v>-0.2912992193387756</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1515260970965627</v>
+        <v>0.1434050287530189</v>
       </c>
       <c r="E55" t="n">
-        <v>0.2405422795004555</v>
+        <v>0.23635273257442</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0.2504521572056835</v>
+        <v>0.5918157153164779</v>
       </c>
       <c r="H55" t="n">
-        <v>0.7886739946230036</v>
+        <v>-0.7767967193471784</v>
       </c>
       <c r="I55" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(b1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_Neu5Ac(a2-?)HexNAc(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.4071610629747092</v>
+        <v>0.1044729828098161</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.2864465407559296</v>
+        <v>-1.476623975536571</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1520669583048856</v>
+        <v>0.1462545352143395</v>
       </c>
       <c r="E56" t="n">
-        <v>0.2405422795004555</v>
+        <v>0.2366664297104766</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>0.6537773533341525</v>
+        <v>0.4107312271350288</v>
       </c>
       <c r="H56" t="n">
-        <v>-0.758729243505552</v>
+        <v>-0.8158438936014987</v>
       </c>
       <c r="I56" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GalNAc</t>
+          <t>Terminal_Neu5Gc(a2-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.5142763151949481</v>
+        <v>0.1824109147640526</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.3833153603115003</v>
+        <v>0.6052000985756241</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1579176267275684</v>
+        <v>0.1648827983994084</v>
       </c>
       <c r="E57" t="n">
-        <v>0.2453363129517581</v>
+        <v>0.2620458760276312</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.7665707750453825</v>
+        <v>0.752847645176814</v>
       </c>
       <c r="I57" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Gc(a2-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_Man(a1-3)Man(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.1817192556849913</v>
+        <v>0.07496147881876188</v>
       </c>
       <c r="C58" t="n">
-        <v>0.6298746305008347</v>
+        <v>0.513786765252077</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1631484392631812</v>
+        <v>0.1709934683385637</v>
       </c>
       <c r="E58" t="n">
-        <v>0.2490160388753818</v>
+        <v>0.2669898014409152</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H58" t="n">
-        <v>0.7588339432352325</v>
+        <v>0.7488097754753857</v>
       </c>
       <c r="I58" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="59">
@@ -2254,245 +2254,245 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.3807054559032345</v>
+        <v>0.3809979054073658</v>
       </c>
       <c r="C59" t="n">
-        <v>0.5927614102120797</v>
+        <v>0.5867183491012646</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1877514648452815</v>
+        <v>0.1757266542386947</v>
       </c>
       <c r="E59" t="n">
-        <v>0.2816271972679223</v>
+        <v>0.2696495211593763</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H59" t="n">
-        <v>0.7142346171371542</v>
+        <v>0.7346342430007462</v>
       </c>
       <c r="I59" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-?)Gal(b1-?)</t>
+          <t>Terminal_Neu5Gc(a2-6)GalNAc</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1.150878892119407</v>
+        <v>0.1255063264322316</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.3317159879001963</v>
+        <v>0.5758408738620147</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1943664636366887</v>
+        <v>0.2005006137540691</v>
       </c>
       <c r="E60" t="n">
-        <v>0.2866081751930833</v>
+        <v>0.2878153971630992</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0.2962786121219571</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H60" t="n">
-        <v>-0.7000583289711433</v>
+        <v>0.6891703644258833</v>
       </c>
       <c r="I60" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-3)</t>
+          <t>Terminal_Gal(b1-3)[Neu5Ac(a2-6)]GalNAc</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.3618265935219169</v>
+        <v>0.03278234707875527</v>
       </c>
       <c r="C61" t="n">
-        <v>0.4406685906424901</v>
+        <v>0.4383026049947281</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2056049832045632</v>
+        <v>0.1994811357975912</v>
       </c>
       <c r="E61" t="n">
-        <v>0.2981272256466166</v>
+        <v>0.2878153971630992</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H61" t="n">
-        <v>0.682494234853245</v>
+        <v>0.6992877189814177</v>
       </c>
       <c r="I61" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)GalNAc</t>
+          <t>Terminal_GlcNAc(a1-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.06097145506295127</v>
+        <v>1.149555728252632</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.9219597450151691</v>
+        <v>-0.3343893588682967</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2097178915512989</v>
+        <v>0.1930880519268653</v>
       </c>
       <c r="E62" t="n">
-        <v>0.2991058453272624</v>
+        <v>0.2878153971630992</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0.73441791497008</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H62" t="n">
-        <v>-0.658981205862424</v>
+        <v>-0.7023208069586031</v>
       </c>
       <c r="I62" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)[Neu5Ac(a2-6)]GalNAc</t>
+          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.03284351740567099</v>
+        <v>0.06047759087912366</v>
       </c>
       <c r="C63" t="n">
-        <v>0.4378614662419197</v>
+        <v>-0.9476028726974961</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2175295858059733</v>
+        <v>0.1945420760537999</v>
       </c>
       <c r="E63" t="n">
-        <v>0.3052431284696721</v>
+        <v>0.2878153971630992</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.7226264087549213</v>
       </c>
       <c r="H63" t="n">
-        <v>0.6697660528882192</v>
+        <v>-0.6827885257458118</v>
       </c>
       <c r="I63" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Gc(a2-3)Gal(b1-3)GalNAc</t>
+          <t>Terminal_Man(a1-2)Man(a1-6)Man</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.07322992545466225</v>
+        <v>0.1039020087978417</v>
       </c>
       <c r="C64" t="n">
-        <v>0.5950396324361533</v>
+        <v>0.3487590888063166</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2223006071837103</v>
+        <v>0.2344894308332229</v>
       </c>
       <c r="E64" t="n">
-        <v>0.3069865527775046</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2509866995169991</v>
       </c>
       <c r="H64" t="n">
-        <v>0.6547723075714751</v>
+        <v>0.6308227238466905</v>
       </c>
       <c r="I64" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-3)[Man(a1-6)]Man</t>
+          <t>Terminal_Man(a1-3)</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.2867225565524934</v>
+        <v>0.3611385239058851</v>
       </c>
       <c r="C65" t="n">
-        <v>0.4130844906869604</v>
+        <v>0.4435295437085998</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2310872222031835</v>
+        <v>0.2155853900409831</v>
       </c>
       <c r="E65" t="n">
-        <v>0.3125922292013846</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H65" t="n">
-        <v>0.6417406946554042</v>
+        <v>0.6671383220734458</v>
       </c>
       <c r="I65" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Gc(a2-6)GalNAc</t>
+          <t>Terminal_Man(a1-2)Man(a1-3)Man</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1257562747635809</v>
+        <v>0.2330531414891961</v>
       </c>
       <c r="C66" t="n">
-        <v>0.5423840008737546</v>
+        <v>0.403858431411162</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2365357152829903</v>
+        <v>0.2219166990523196</v>
       </c>
       <c r="E66" t="n">
-        <v>0.3125922292013846</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H66" t="n">
-        <v>0.6333679442914883</v>
+        <v>0.6543916286274872</v>
       </c>
       <c r="I66" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="67">
@@ -2502,183 +2502,183 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1.17243116778437</v>
+        <v>1.170237161654895</v>
       </c>
       <c r="C67" t="n">
-        <v>0.3904886448370313</v>
+        <v>0.4063844107584105</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2371389324976021</v>
+        <v>0.2270662301194186</v>
       </c>
       <c r="E67" t="n">
-        <v>0.3125922292013846</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H67" t="n">
-        <v>0.6317971428461371</v>
+        <v>0.6472080617345219</v>
       </c>
       <c r="I67" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-?)Man(a1-?)Man</t>
+          <t>Terminal_Neu5Gc(a2-3)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1.097327130814947</v>
+        <v>0.07308066421108161</v>
       </c>
       <c r="C68" t="n">
-        <v>0.3794785025477125</v>
+        <v>0.5537466699364874</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2485554387284882</v>
+        <v>0.2323047115220472</v>
       </c>
       <c r="E68" t="n">
-        <v>0.3227510920802757</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H68" t="n">
-        <v>0.6152051601908161</v>
+        <v>0.6386005509155405</v>
       </c>
       <c r="I68" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-2)Man(a1-3)Man</t>
+          <t>Terminal_Man(a1-3)[Man(a1-6)]Man</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.2334898348898195</v>
+        <v>0.2861770450871232</v>
       </c>
       <c r="C69" t="n">
-        <v>0.3827443637795365</v>
+        <v>0.4242505341877187</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2538661775723363</v>
+        <v>0.2325613396984123</v>
       </c>
       <c r="E69" t="n">
-        <v>0.3247993742469597</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H69" t="n">
-        <v>0.608309422561585</v>
+        <v>0.6402949780318354</v>
       </c>
       <c r="I69" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)</t>
+          <t>Terminal_Man(a1-?)Man(a1-?)Man</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.4016297536651197</v>
+        <v>1.095275682836133</v>
       </c>
       <c r="C70" t="n">
-        <v>0.3740946124564775</v>
+        <v>0.3985274001372794</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2585971295322702</v>
+        <v>0.2337406649012952</v>
       </c>
       <c r="E70" t="n">
-        <v>0.3260572502798189</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>0.2775056820658957</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H70" t="n">
-        <v>0.5933769935712343</v>
+        <v>0.6368968635730773</v>
       </c>
       <c r="I70" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)Gal</t>
+          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.5459063506537984</v>
+        <v>0.4006075701194006</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.2682964378801991</v>
+        <v>0.3894431892510615</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2692632075602692</v>
+        <v>0.2372512106819264</v>
       </c>
       <c r="E71" t="n">
-        <v>0.3326803125436615</v>
+        <v>0.3016479678670207</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>0.2885098853140555</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H71" t="n">
-        <v>-0.5817238423663935</v>
+        <v>0.622151261129699</v>
       </c>
       <c r="I71" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-2)Man(a1-6)Man</t>
+          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.1040878327089633</v>
+        <v>0.1979048474966604</v>
       </c>
       <c r="C72" t="n">
-        <v>0.3272602220382022</v>
+        <v>-0.2505055694345391</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2714977263287353</v>
+        <v>0.2459756574876364</v>
       </c>
       <c r="E72" t="n">
-        <v>0.3326803125436615</v>
+        <v>0.3040532432833283</v>
       </c>
       <c r="F72" t="b">
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.4657318171624223</v>
       </c>
       <c r="H72" t="n">
-        <v>0.5808311817119765</v>
+        <v>-0.6060623038181044</v>
       </c>
       <c r="I72" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="73">
@@ -2688,524 +2688,524 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.5238820177099598</v>
+        <v>0.5229215926618864</v>
       </c>
       <c r="C73" t="n">
-        <v>0.342196105282389</v>
+        <v>0.3678957456744505</v>
       </c>
       <c r="D73" t="n">
-        <v>0.2756574340454399</v>
+        <v>0.2427694336114063</v>
       </c>
       <c r="E73" t="n">
-        <v>0.3330860661382399</v>
+        <v>0.3040532432833283</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H73" t="n">
-        <v>0.57731644902224</v>
+        <v>0.6216214238739474</v>
       </c>
       <c r="I73" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)</t>
+          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)Gal</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.4537603508857209</v>
+        <v>0.5446953724960576</v>
       </c>
       <c r="C74" t="n">
-        <v>0.3260287716574974</v>
+        <v>-0.2977883366528968</v>
       </c>
       <c r="D74" t="n">
-        <v>0.28696311767775</v>
+        <v>0.2523731285886694</v>
       </c>
       <c r="E74" t="n">
-        <v>0.3419971402460856</v>
+        <v>0.3076877869094737</v>
       </c>
       <c r="F74" t="b">
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H74" t="n">
-        <v>0.5596818247014974</v>
+        <v>-0.6054499332414203</v>
       </c>
       <c r="I74" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Terminal_Gal(a1-?)Gal(b1-?)</t>
+          <t>Terminal_Neu5Ac(a2-3)</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.1684608004010061</v>
+        <v>0.4525980419727241</v>
       </c>
       <c r="C75" t="n">
-        <v>0.2182808604905602</v>
+        <v>0.3340489789303565</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2915908500949774</v>
+        <v>0.2768827465907133</v>
       </c>
       <c r="E75" t="n">
-        <v>0.3428162697062572</v>
+        <v>0.3293287088906414</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>0.823958810172822</v>
+        <v>0.2740857702405718</v>
       </c>
       <c r="H75" t="n">
-        <v>0.5479815139581971</v>
+        <v>0.5721081704665474</v>
       </c>
       <c r="I75" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(b1-?)[Fuc(a1-?)]GlcNAc</t>
+          <t>Terminal_Man(?1-?)</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.05474625123538936</v>
+        <v>0.2376682228978685</v>
       </c>
       <c r="C76" t="n">
-        <v>-1.183821381203247</v>
+        <v>0.380888484185486</v>
       </c>
       <c r="D76" t="n">
-        <v>0.3086873436998439</v>
+        <v>0.2821427942488373</v>
       </c>
       <c r="E76" t="n">
-        <v>0.3536867233898641</v>
+        <v>0.3293287088906414</v>
       </c>
       <c r="F76" t="b">
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>0.7136332712011645</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H76" t="n">
-        <v>-0.529646773502659</v>
+        <v>0.5703075663013011</v>
       </c>
       <c r="I76" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-6)GalNAc</t>
+          <t>Terminal_Neu5Ac(a2-3)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.1780469234212597</v>
+        <v>0.1025483434033696</v>
       </c>
       <c r="C77" t="n">
-        <v>0.3621657316299931</v>
+        <v>0.5842581253149861</v>
       </c>
       <c r="D77" t="n">
-        <v>0.3126220808810637</v>
+        <v>0.2843289879321326</v>
       </c>
       <c r="E77" t="n">
-        <v>0.3536867233898641</v>
+        <v>0.3293287088906414</v>
       </c>
       <c r="F77" t="b">
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.6930437404444199</v>
       </c>
       <c r="H77" t="n">
-        <v>0.5347156394892627</v>
+        <v>0.5567069542055616</v>
       </c>
       <c r="I77" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Terminal_Man(?1-?)</t>
+          <t>Terminal_Man(a1-2)Man(a1-2)Man</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.2381201080404819</v>
+        <v>0.1859664423748486</v>
       </c>
       <c r="C78" t="n">
-        <v>0.3405112848577279</v>
+        <v>0.3323389916637589</v>
       </c>
       <c r="D78" t="n">
-        <v>0.313033077023213</v>
+        <v>0.2849248380289819</v>
       </c>
       <c r="E78" t="n">
-        <v>0.3536867233898641</v>
+        <v>0.3293287088906414</v>
       </c>
       <c r="F78" t="b">
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.2740857702405718</v>
       </c>
       <c r="H78" t="n">
-        <v>0.532067550848012</v>
+        <v>0.5645597036172695</v>
       </c>
       <c r="I78" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-2)Man(a1-2)Man</t>
+          <t>Terminal_GalNAc(b1-?)[Fuc(a1-?)]GlcNAc</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.1863043501111769</v>
+        <v>0.05426102621222016</v>
       </c>
       <c r="C79" t="n">
-        <v>0.2967554905640553</v>
+        <v>-1.239379967819038</v>
       </c>
       <c r="D79" t="n">
-        <v>0.3218791699299709</v>
+        <v>0.2930803355439516</v>
       </c>
       <c r="E79" t="n">
-        <v>0.3590190741526599</v>
+        <v>0.3344121777360474</v>
       </c>
       <c r="F79" t="b">
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.6917083001501491</v>
       </c>
       <c r="H79" t="n">
-        <v>0.5201537830777934</v>
+        <v>-0.547979074993341</v>
       </c>
       <c r="I79" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_Gal(a1-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.02975107082429825</v>
+        <v>0.1678123651006547</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.1846385570209045</v>
+        <v>0.2155238792188221</v>
       </c>
       <c r="D80" t="n">
-        <v>0.3270815254663166</v>
+        <v>0.3058513193400985</v>
       </c>
       <c r="E80" t="n">
-        <v>0.360203705260374</v>
+        <v>0.3445666762185919</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0.5556987528519068</v>
+        <v>0.9147432125301069</v>
       </c>
       <c r="H80" t="n">
-        <v>-0.5098295526066261</v>
+        <v>0.5314587457965577</v>
       </c>
       <c r="I80" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.1027489660290588</v>
+        <v>0.4079084037061881</v>
       </c>
       <c r="C81" t="n">
-        <v>0.5416109658422894</v>
+        <v>-0.2611864621500093</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3318595649569248</v>
+        <v>0.313564462117053</v>
       </c>
       <c r="E81" t="n">
-        <v>0.3608972768906557</v>
+        <v>0.3450279372509686</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>0.7727143972181569</v>
+        <v>0.4605765235170522</v>
       </c>
       <c r="H81" t="n">
-        <v>0.5025995525688672</v>
+        <v>-0.5250542411514602</v>
       </c>
       <c r="I81" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)GalNAc</t>
+          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)Gal</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.01013341142407019</v>
+        <v>0.3977919819503951</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.2858605274235011</v>
+        <v>-0.2618544818891069</v>
       </c>
       <c r="D82" t="n">
-        <v>0.3502143726744392</v>
+        <v>0.3140141900823422</v>
       </c>
       <c r="E82" t="n">
-        <v>0.376156178057731</v>
+        <v>0.3450279372509686</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.3999526768896021</v>
+        <v>0.4657318171624223</v>
       </c>
       <c r="H82" t="n">
-        <v>-0.4848759975460781</v>
+        <v>-0.5245448925396637</v>
       </c>
       <c r="I82" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-6)GalNAc</t>
+          <t>Terminal_Neu5Ac(a2-6)GalNAc</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.1981912329635399</v>
+        <v>0.177706979136253</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.1828621573811171</v>
+        <v>0.3329767379339656</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3918773049074444</v>
+        <v>0.3454045136449195</v>
       </c>
       <c r="E83" t="n">
-        <v>0.4110321731785382</v>
+        <v>0.3659643061237838</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>0.5292082949514116</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H83" t="n">
-        <v>-0.4420636950205157</v>
+        <v>0.4976453471475981</v>
       </c>
       <c r="I83" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)</t>
+          <t>Terminal_GlcNAc(a1-4)</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.2832778932056133</v>
+        <v>2.079171830152811</v>
       </c>
       <c r="C84" t="n">
-        <v>0.3261480060657056</v>
+        <v>-0.2549194473555003</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3932918751713903</v>
+        <v>0.3452239990011371</v>
       </c>
       <c r="E84" t="n">
-        <v>0.4110321731785382</v>
+        <v>0.3659643061237838</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H84" t="n">
-        <v>0.4481175492144349</v>
+        <v>-0.4944686271171146</v>
       </c>
       <c r="I84" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-4)</t>
+          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>2.081925273086522</v>
+        <v>0.1181849500849922</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.2295061619858236</v>
+        <v>0.3804638212796156</v>
       </c>
       <c r="D85" t="n">
-        <v>0.3968586499654851</v>
+        <v>0.3446298184401125</v>
       </c>
       <c r="E85" t="n">
-        <v>0.4110321731785382</v>
+        <v>0.3659643061237838</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>0.2775056820658957</v>
+        <v>0.4971996293476879</v>
       </c>
       <c r="H85" t="n">
-        <v>-0.442003872871389</v>
+        <v>0.4901601490897356</v>
       </c>
       <c r="I85" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_Gal(?1-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.1183518604595064</v>
+        <v>0.02970489775090981</v>
       </c>
       <c r="C86" t="n">
-        <v>0.3358247569319281</v>
+        <v>-0.163820179444903</v>
       </c>
       <c r="D86" t="n">
-        <v>0.4128278435229761</v>
+        <v>0.3840368670834285</v>
       </c>
       <c r="E86" t="n">
-        <v>0.4225414398411638</v>
+        <v>0.4021091902402958</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0.5556987528519068</v>
+        <v>0.469782273628425</v>
       </c>
       <c r="H86" t="n">
-        <v>0.4225369281750155</v>
+        <v>-0.4510234632461436</v>
       </c>
       <c r="I86" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)</t>
+          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.4089172841011298</v>
+        <v>0.2824226200344084</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.1986755149478299</v>
+        <v>0.3278465752467707</v>
       </c>
       <c r="D87" t="n">
-        <v>0.4362830781906997</v>
+        <v>0.3931043893024516</v>
       </c>
       <c r="E87" t="n">
-        <v>0.4411391962108507</v>
+        <v>0.4068173331153279</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>0.4900435232578885</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H87" t="n">
-        <v>-0.402141282750518</v>
+        <v>0.448234189732682</v>
       </c>
       <c r="I87" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)Gal</t>
+          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.3987838726770597</v>
+        <v>0.01011642175579304</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.1961489934555991</v>
+        <v>-0.2248104380115976</v>
       </c>
       <c r="D88" t="n">
-        <v>0.441809652987788</v>
+        <v>0.4083234061562022</v>
       </c>
       <c r="E88" t="n">
-        <v>0.441809652987788</v>
+        <v>0.4177101511253103</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>0.5013935247770087</v>
+        <v>0.5970596995326609</v>
       </c>
       <c r="H88" t="n">
-        <v>-0.397154838490686</v>
+        <v>-0.4264774943400428</v>
       </c>
       <c r="I88" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)GalNAc</t>
+          <t>Terminal_Gal(a1-3)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.3244844519550276</v>
+        <v>0.08827716814276533</v>
       </c>
       <c r="C89" t="n">
-        <v>0.2665133689755481</v>
+        <v>-0.1783248620417563</v>
       </c>
       <c r="D89" t="n">
-        <v>0.4462097616845386</v>
+        <v>0.4303907122973775</v>
       </c>
       <c r="E89" t="n">
-        <v>0.4462097616845386</v>
+        <v>0.4326640340391278</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H89" t="n">
-        <v>0.399194815676391</v>
+        <v>-0.4090338653001283</v>
       </c>
       <c r="I89" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="90">
@@ -3215,245 +3215,245 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.009453055016333796</v>
+        <v>0.009413063805027024</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.8350324661379132</v>
+        <v>-0.9346180086464733</v>
       </c>
       <c r="D90" t="n">
-        <v>0.4852955926985744</v>
+        <v>0.4326640340391278</v>
       </c>
       <c r="E90" t="n">
-        <v>0.4852955926985744</v>
+        <v>0.4326640340391278</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>0.8041092304907818</v>
+        <v>0.8238196446891592</v>
       </c>
       <c r="H90" t="n">
-        <v>-0.3586073672714595</v>
+        <v>-0.4042643746793285</v>
       </c>
       <c r="I90" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-4)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.600165890501179</v>
+        <v>0.3235662174643425</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.2114944450277179</v>
+        <v>0.2675802158585641</v>
       </c>
       <c r="D91" t="n">
-        <v>0.4924487567529862</v>
+        <v>0.4451997358113917</v>
       </c>
       <c r="E91" t="n">
-        <v>0.4924487567529862</v>
+        <v>0.4451997358113917</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>0.2775056820658957</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H91" t="n">
-        <v>-0.3570920768925693</v>
+        <v>0.4000590347334048</v>
       </c>
       <c r="I91" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Terminal_Gal(a1-3)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_GlcNAc(a1-4)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.08877628546353833</v>
+        <v>0.5992605103246086</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.1499598205664479</v>
+        <v>-0.2226930471236086</v>
       </c>
       <c r="D92" t="n">
-        <v>0.5153713703901945</v>
+        <v>0.4538656612430946</v>
       </c>
       <c r="E92" t="n">
-        <v>0.5153713703901945</v>
+        <v>0.4538656612430946</v>
       </c>
       <c r="F92" t="b">
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>0.3161976169782357</v>
+        <v>0.3077533846388161</v>
       </c>
       <c r="H92" t="n">
-        <v>-0.3354693611638405</v>
+        <v>-0.3902335456001609</v>
       </c>
       <c r="I92" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)[GalNAc(b1-4)]Gal</t>
+          <t>Terminal_GlcNAc(a1-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.04120655874941433</v>
+        <v>0.929616101900179</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.08755735888571016</v>
+        <v>-0.1506195041323002</v>
       </c>
       <c r="D93" t="n">
-        <v>0.740649077745009</v>
+        <v>0.6229845839920392</v>
       </c>
       <c r="E93" t="n">
-        <v>0.740649077745009</v>
+        <v>0.6229845839920392</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>0.2582556565856777</v>
+        <v>0.3196999040457143</v>
       </c>
       <c r="H93" t="n">
-        <v>-0.1697134665098624</v>
+        <v>-0.2522462042682229</v>
       </c>
       <c r="I93" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_Neu5Ac(a2-3)[GalNAc(b1-4)]Gal</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.9310463809671153</v>
+        <v>0.04114359742993404</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.09745860337545764</v>
+        <v>-0.09988655891336165</v>
       </c>
       <c r="D94" t="n">
-        <v>0.751682078739432</v>
+        <v>0.7103360285421068</v>
       </c>
       <c r="E94" t="n">
-        <v>0.751682078739432</v>
+        <v>0.7103360285421068</v>
       </c>
       <c r="F94" t="b">
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>0.2967971322525303</v>
+        <v>0.2740857702405718</v>
       </c>
       <c r="H94" t="n">
-        <v>-0.1618897496974479</v>
+        <v>-0.1906079263239622</v>
       </c>
       <c r="I94" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(b1-4)Man(b1-4)GlcNAc</t>
+          <t>Terminal_Neu5Ac(a2-?)</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.01361501185025847</v>
+        <v>1.194959937523557</v>
       </c>
       <c r="C95" t="n">
-        <v>0.2655186737679531</v>
+        <v>-0.03541860903789118</v>
       </c>
       <c r="D95" t="n">
-        <v>0.8108576008042536</v>
+        <v>0.7918182653159127</v>
       </c>
       <c r="E95" t="n">
-        <v>0.8108576008042536</v>
+        <v>0.7918182653159127</v>
       </c>
       <c r="F95" t="b">
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0.9912269033752943</v>
+        <v>0.7945991714548725</v>
       </c>
       <c r="H95" t="n">
-        <v>0.1220014575013231</v>
+        <v>-0.1345242827016563</v>
       </c>
       <c r="I95" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)</t>
+          <t>Terminal_Gal(b1-3)[Neu5Gc(a2-6)]GalNAc</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>1.179693963409588</v>
+        <v>0.003677336218008109</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.01659759543547423</v>
+        <v>0.07766276802773842</v>
       </c>
       <c r="D96" t="n">
-        <v>0.9006554913900165</v>
+        <v>0.8168300463850234</v>
       </c>
       <c r="E96" t="n">
-        <v>0.9006554913900165</v>
+        <v>0.8168300463850234</v>
       </c>
       <c r="F96" t="b">
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>0.8041092304907818</v>
+        <v>0.2373900366976995</v>
       </c>
       <c r="H96" t="n">
-        <v>-0.06355997752780215</v>
+        <v>0.1191495396570765</v>
       </c>
       <c r="I96" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)[Neu5Gc(a2-6)]GalNAc</t>
+          <t>Terminal_GlcNAc(b1-4)Man(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.003684398148511174</v>
+        <v>0.01359573569291573</v>
       </c>
       <c r="C97" t="n">
-        <v>0.03170205009360716</v>
+        <v>0.1714082149092633</v>
       </c>
       <c r="D97" t="n">
-        <v>0.9318422665523242</v>
+        <v>0.8764858741655575</v>
       </c>
       <c r="E97" t="n">
-        <v>0.9318422665523242</v>
+        <v>0.8764858741655575</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>0.2215868623311513</v>
+        <v>0.8736354495724126</v>
       </c>
       <c r="H97" t="n">
-        <v>0.04399681149086491</v>
+        <v>0.07917543713819847</v>
       </c>
       <c r="I97" t="n">
-        <v>0.9523706226862587</v>
+        <v>0.9467929378407232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run 2025-05-08 in fresh install
Running through the entire script on a fresh install for manuscript submission.
</commit_message>
<xml_diff>
--- a/Python_output_files/Tables/differential_glycomics_cohort.xlsx
+++ b/Python_output_files/Tables/differential_glycomics_cohort.xlsx
@@ -487,25 +487,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.443509489723976</v>
+        <v>2.446040337206336</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.5100129492086909</v>
+        <v>-0.487962648816147</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0004428358820680877</v>
+        <v>0.0006677543174440321</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03648684383893259</v>
+        <v>0.03034679005579992</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.975528284353872</v>
+        <v>0.8463360188704392</v>
       </c>
       <c r="H2" t="n">
-        <v>-2.305474321112631</v>
+        <v>-2.197037062287912</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -514,29 +514,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Man</t>
+          <t>Terminal_Fuc(a1-3)GlcNAc(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.04358315409335117</v>
+        <v>0.006223652409671476</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.685319430820699</v>
+        <v>-0.481004270987607</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001215295417290745</v>
+        <v>0.0006976273576045958</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03648684383893259</v>
+        <v>0.03034679005579992</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5909631192162319</v>
+        <v>0.8516431490018207</v>
       </c>
       <c r="H3" t="n">
-        <v>-2.051703276277024</v>
+        <v>-2.162983302464875</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -545,29 +545,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)Gal(b1-3)GalNAc</t>
+          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Man</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.27417043897451</v>
+        <v>0.04361157731016907</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4647369312423208</v>
+        <v>-0.6691560827737829</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001345064420685694</v>
+        <v>0.001220141840034913</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03648684383893259</v>
+        <v>0.03221317702346361</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3436622619306631</v>
+        <v>0.5508458305351739</v>
       </c>
       <c r="H4" t="n">
-        <v>-2.176904798617128</v>
+        <v>-2.04414079135608</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -580,25 +580,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.56639854149799</v>
+        <v>10.57344253200534</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.5692080704595535</v>
+        <v>-0.5530610980490573</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001987430157832661</v>
+        <v>0.001957289441368687</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03648684383893259</v>
+        <v>0.03221317702346361</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2459943196847548</v>
+        <v>0.2691002775158839</v>
       </c>
       <c r="H5" t="n">
-        <v>-1.980568502369943</v>
+        <v>-1.973820983429243</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -607,29 +607,29 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)</t>
+          <t>Terminal_Fuc(a1-2)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12.02614815637013</v>
+        <v>2.276626501519323</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.5692074062700723</v>
+        <v>-0.4335631289057718</v>
       </c>
       <c r="D6" t="n">
-        <v>0.002508464213879337</v>
+        <v>0.002273629616690133</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03648684383893259</v>
+        <v>0.03221317702346361</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.3000955164596797</v>
       </c>
       <c r="H6" t="n">
-        <v>-1.939590768392043</v>
+        <v>-1.999062354921012</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
@@ -638,29 +638,29 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)</t>
+          <t>Terminal_Fuc(a1-2)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12.47435014356301</v>
+        <v>12.02489351772718</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.5680940361163405</v>
+        <v>-0.5553324627340706</v>
       </c>
       <c r="D7" t="n">
-        <v>0.002545593756204599</v>
+        <v>0.002411064940169871</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03648684383893259</v>
+        <v>0.03221317702346361</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.934805237718694</v>
+        <v>-1.939636410544491</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -669,29 +669,29 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)[Gal(a1-3)]Gal</t>
+          <t>Terminal_Fuc(a1-?)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05534651790408739</v>
+        <v>12.47019891737128</v>
       </c>
       <c r="C8" t="n">
-        <v>1.385378758621724</v>
+        <v>-0.5529541297557845</v>
       </c>
       <c r="D8" t="n">
-        <v>0.003102852663871817</v>
+        <v>0.002591864817979831</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03812076129899661</v>
+        <v>0.03221317702346361</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5065349861342567</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H8" t="n">
-        <v>1.922925894418983</v>
+        <v>-1.920572529602846</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -700,29 +700,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_Fuc(a1-2)[Gal(a1-3)]Gal</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8.341355521445738</v>
+        <v>0.05541711297761647</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.5858819953113041</v>
+        <v>1.399843387181765</v>
       </c>
       <c r="D9" t="n">
-        <v>0.004095865416389856</v>
+        <v>0.003477713172701158</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04306443881463076</v>
+        <v>0.0378201307531251</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2065214492646669</v>
+        <v>0.4020216519427967</v>
       </c>
       <c r="H9" t="n">
-        <v>-1.796137406391547</v>
+        <v>1.89844092011139</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
@@ -731,29 +731,29 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-3)GlcNAc(b1-6)GalNAc</t>
+          <t>Terminal_Fuc(a1-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.006219098981833053</v>
+        <v>8.346009491053966</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.4461199783305356</v>
+        <v>-0.5739999852552442</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0045590614878796</v>
+        <v>0.003936529768386937</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04306443881463076</v>
+        <v>0.03805312109440705</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6397666871592189</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H10" t="n">
-        <v>-1.708324373354246</v>
+        <v>-1.800207297158315</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -766,25 +766,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2419349751069767</v>
+        <v>0.2421149605868468</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.5070251312562277</v>
+        <v>-0.5650752614254384</v>
       </c>
       <c r="D11" t="n">
-        <v>0.005007492885422182</v>
+        <v>0.005966714919982703</v>
       </c>
       <c r="E11" t="n">
-        <v>0.04306443881463076</v>
+        <v>0.04955952771726518</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8426582200271998</v>
+        <v>0.5389670244540066</v>
       </c>
       <c r="H11" t="n">
-        <v>-1.720137246987448</v>
+        <v>-1.708242880643364</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -797,25 +797,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6.604263907299336</v>
+        <v>6.60782412976675</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.556291077263154</v>
+        <v>-0.5425174036832487</v>
       </c>
       <c r="D12" t="n">
-        <v>0.005875607856913966</v>
+        <v>0.006266147182642724</v>
       </c>
       <c r="E12" t="n">
-        <v>0.04593657051769101</v>
+        <v>0.04955952771726518</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2410350884517359</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.697565301824496</v>
+        <v>-1.676304422241701</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
@@ -828,25 +828,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.03696127613577115</v>
+        <v>0.0370151767767828</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8656048271266689</v>
+        <v>0.90844926983426</v>
       </c>
       <c r="D13" t="n">
-        <v>0.007476573581393703</v>
+        <v>0.006838101239543292</v>
       </c>
       <c r="E13" t="n">
-        <v>0.05232678278200197</v>
+        <v>0.04957623398668887</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5909631192162319</v>
+        <v>0.7440563430518369</v>
       </c>
       <c r="H13" t="n">
-        <v>1.570293238395555</v>
+        <v>1.587157234328274</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
@@ -855,29 +855,29 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)[Fuc(a1-?)]GalNAc</t>
+          <t>Terminal_HexNAc(?1-?)GlcNAc(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01654482821670868</v>
+        <v>0.0922298591223589</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.5408312341924959</v>
+        <v>-0.7926739451573226</v>
       </c>
       <c r="D14" t="n">
-        <v>0.007909862513558436</v>
+        <v>0.009003406668353539</v>
       </c>
       <c r="E14" t="n">
-        <v>0.05232678278200197</v>
+        <v>0.04992828083435227</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3892258307000309</v>
+        <v>0.2639442526448085</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.622035101683706</v>
+        <v>-1.561657697960316</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -886,29 +886,29 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)GlcNAc(b1-?)GalNAc</t>
+          <t>Terminal_Gal(b1-?)[Fuc(a1-?)]GalNAc</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.09217885166924601</v>
+        <v>0.01655726858977495</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.8276083733078977</v>
+        <v>-0.5431080807179065</v>
       </c>
       <c r="D15" t="n">
-        <v>0.008876305829598113</v>
+        <v>0.009069282867319806</v>
       </c>
       <c r="E15" t="n">
-        <v>0.05452587866753127</v>
+        <v>0.04992828083435227</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3004829382090763</v>
+        <v>0.401701710662534</v>
       </c>
       <c r="H15" t="n">
-        <v>-1.574317263196881</v>
+        <v>-1.592610044681535</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
@@ -917,29 +917,29 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(b1-6)GalNAc</t>
+          <t>Terminal_Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.8672891537723419</v>
+        <v>0.6920614097708702</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.4543699584223253</v>
+        <v>-0.4610051385351976</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01157462488098992</v>
+        <v>0.009341880453357529</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05700633803651601</v>
+        <v>0.04992828083435227</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.8129643318725018</v>
       </c>
       <c r="H16" t="n">
-        <v>-1.494085694079505</v>
+        <v>-1.560600184919827</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -952,25 +952,25 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.146783488996461</v>
+        <v>1.147712279295668</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.5049573324215615</v>
+        <v>-0.5526166495127773</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01175573582081077</v>
+        <v>0.00954012823700311</v>
       </c>
       <c r="E17" t="n">
-        <v>0.05700633803651601</v>
+        <v>0.04992828083435227</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0.650792087649344</v>
+        <v>0.5508458305351739</v>
       </c>
       <c r="H17" t="n">
-        <v>-1.522654660389702</v>
+        <v>-1.593771355034473</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
@@ -983,25 +983,25 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.156904369872038</v>
+        <v>1.157843328694545</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.5037654065844803</v>
+        <v>-0.550425005347388</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01182130350570266</v>
+        <v>0.009756100852689525</v>
       </c>
       <c r="E18" t="n">
-        <v>0.05700633803651601</v>
+        <v>0.04992828083435227</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>0.650792087649344</v>
+        <v>0.5508458305351739</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.522383664986168</v>
+        <v>-1.588975757611798</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
@@ -1010,29 +1010,29 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(b1-?)</t>
+          <t>Terminal_Gal(b1-3)</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8836017870351877</v>
+        <v>1.008451624784181</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.4331036312792902</v>
+        <v>-0.4204479626531628</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01193155912392196</v>
+        <v>0.01052819034240714</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05700633803651601</v>
+        <v>0.05088625332163449</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4622211408912558</v>
+        <v>0.6685606376089005</v>
       </c>
       <c r="H19" t="n">
-        <v>-1.474687171431136</v>
+        <v>-1.540740117152668</v>
       </c>
       <c r="I19" t="n">
         <v>1</v>
@@ -1041,29 +1041,29 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)Gal(?1-?)</t>
+          <t>Terminal_GlcNAc(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.435772820819669</v>
+        <v>0.8656808065373209</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.6733889112847802</v>
+        <v>-0.5039623341783894</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01464936378766982</v>
+        <v>0.01219323702298092</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06154940233919294</v>
+        <v>0.05362394369953043</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2691002775158839</v>
       </c>
       <c r="H20" t="n">
-        <v>-1.533282645334126</v>
+        <v>-1.502729392075452</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
@@ -1072,29 +1072,29 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.426338939084949</v>
+        <v>0.8792753713506855</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.6722734353214923</v>
+        <v>-0.489966377162145</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01468968348197696</v>
+        <v>0.01285186357820288</v>
       </c>
       <c r="E21" t="n">
-        <v>0.06154940233919294</v>
+        <v>0.05362394369953043</v>
       </c>
       <c r="F21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.3003363301440668</v>
       </c>
       <c r="H21" t="n">
-        <v>-1.532616236606485</v>
+        <v>-1.480769872257119</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
@@ -1103,29 +1103,29 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)</t>
+          <t>Terminal_Fuc(a1-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.007553291942021</v>
+        <v>1.41804378041561</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.3890721765975425</v>
+        <v>-0.6796272370097443</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01566768071556907</v>
+        <v>0.0135302836203396</v>
       </c>
       <c r="E22" t="n">
-        <v>0.06154940233919294</v>
+        <v>0.05362394369953043</v>
       </c>
       <c r="F22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7315913230211807</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H22" t="n">
-        <v>-1.428899332772051</v>
+        <v>-1.55492444216582</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
@@ -1134,29 +1134,29 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)GalNAc</t>
+          <t>Terminal_Fuc(a1-?)Gal(?1-?)</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.691434837527819</v>
+        <v>1.427506191059116</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.4251167694435529</v>
+        <v>-0.6805322075552755</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0157451959472354</v>
+        <v>0.01356007771712264</v>
       </c>
       <c r="E23" t="n">
-        <v>0.06154940233919294</v>
+        <v>0.05362394369953043</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>0.7315913230211807</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H23" t="n">
-        <v>-1.420110300973172</v>
+        <v>-1.554038680353146</v>
       </c>
       <c r="I23" t="n">
         <v>1</v>
@@ -1165,29 +1165,29 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(a1-3)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_Gal(b1-?)</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.05459396315189878</v>
+        <v>2.712151703301654</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.7133844261808679</v>
+        <v>-0.4448956805288882</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02622956802442336</v>
+        <v>0.02032071813346343</v>
       </c>
       <c r="E24" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.0768653251135356</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2130591240282091</v>
+        <v>0.401701710662534</v>
       </c>
       <c r="H24" t="n">
-        <v>-1.263208316809199</v>
+        <v>-1.384407159945611</v>
       </c>
       <c r="I24" t="n">
         <v>1</v>
@@ -1196,29 +1196,29 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Gal</t>
+          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.8921739523432944</v>
+        <v>1.94581503910432</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.5705983968116728</v>
+        <v>-0.4723708132325424</v>
       </c>
       <c r="D25" t="n">
-        <v>0.02593451530421473</v>
+        <v>0.02178925260950531</v>
       </c>
       <c r="E25" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.07898604070945675</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0.9996130345372205</v>
+        <v>0.343590919901809</v>
       </c>
       <c r="H25" t="n">
-        <v>-1.285415655898891</v>
+        <v>-1.37032539031136</v>
       </c>
       <c r="I25" t="n">
         <v>1</v>
@@ -1227,29 +1227,29 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-3)GlcNAc(b1-3)Gal</t>
+          <t>Terminal_GlcNAc(a1-4)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.2594793086308226</v>
+        <v>0.5505923932139191</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.5070976111797556</v>
+        <v>-0.4738250335751641</v>
       </c>
       <c r="D26" t="n">
-        <v>0.02579837648421038</v>
+        <v>0.02288957082151277</v>
       </c>
       <c r="E26" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.07965570645886443</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.4020216519427967</v>
       </c>
       <c r="H26" t="n">
-        <v>-1.282878241109429</v>
+        <v>-1.343912435085339</v>
       </c>
       <c r="I26" t="n">
         <v>1</v>
@@ -1258,29 +1258,29 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_Gal(b1-4)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.844360283066377</v>
+        <v>1.556609285519831</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.5007515666759321</v>
+        <v>-0.4630016172845943</v>
       </c>
       <c r="D27" t="n">
-        <v>0.02485430394117223</v>
+        <v>0.02599175636340991</v>
       </c>
       <c r="E27" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.08697241552371777</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.8790855506262389</v>
+        <v>0.3274739676035979</v>
       </c>
       <c r="H27" t="n">
-        <v>-1.304894555650218</v>
+        <v>-1.314121746111587</v>
       </c>
       <c r="I27" t="n">
         <v>1</v>
@@ -1289,29 +1289,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-3)</t>
+          <t>Terminal_Fuc(a1-6)GlcNAc</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.2656984076126557</v>
+        <v>0.06618892970521743</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.5055226885271984</v>
+        <v>-0.6829235371771434</v>
       </c>
       <c r="D28" t="n">
-        <v>0.02469262655816455</v>
+        <v>0.02810045562502137</v>
       </c>
       <c r="E28" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.09054591256951332</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H28" t="n">
-        <v>-1.295460011512318</v>
+        <v>-1.325754150990167</v>
       </c>
       <c r="I28" t="n">
         <v>1</v>
@@ -1320,29 +1320,29 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)GalNAc</t>
+          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)Gal</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.02666570909228576</v>
+        <v>0.8928681842209547</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.4629182819529731</v>
+        <v>-0.5711076049614254</v>
       </c>
       <c r="D29" t="n">
-        <v>0.02442090940842242</v>
+        <v>0.0340017351603017</v>
       </c>
       <c r="E29" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.10477736138063</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0.659511491004663</v>
+        <v>0.9215623702504208</v>
       </c>
       <c r="H29" t="n">
-        <v>-1.287712815296742</v>
+        <v>-1.217172752787546</v>
       </c>
       <c r="I29" t="n">
         <v>1</v>
@@ -1351,29 +1351,29 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)</t>
+          <t>Terminal_Fuc(a1-?)GalNAc</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1.55475041583068</v>
+        <v>0.02668831798865179</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.4551853867199132</v>
+        <v>-0.4305120741271417</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01989727363423895</v>
+        <v>0.03492578712687665</v>
       </c>
       <c r="E30" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.10477736138063</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.4081714444217342</v>
+        <v>0.5240530363668825</v>
       </c>
       <c r="H30" t="n">
-        <v>-1.380991147886791</v>
+        <v>-1.191749797035487</v>
       </c>
       <c r="I30" t="n">
         <v>1</v>
@@ -1382,29 +1382,29 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_Gal(?1-?)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3140643340782019</v>
+        <v>1.882678882228277</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.5438839907180553</v>
+        <v>-0.4808971751900906</v>
       </c>
       <c r="D31" t="n">
-        <v>0.02317009942412466</v>
+        <v>0.03774014725463596</v>
       </c>
       <c r="E31" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.1071194811008229</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.598344305654578</v>
+        <v>0.77457885796807</v>
       </c>
       <c r="H31" t="n">
-        <v>-1.285245836332289</v>
+        <v>-1.192566145515212</v>
       </c>
       <c r="I31" t="n">
         <v>1</v>
@@ -1413,29 +1413,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)</t>
+          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2.70925670336863</v>
+        <v>1.843475920559738</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.4248686950304661</v>
+        <v>-0.4871195149198142</v>
       </c>
       <c r="D32" t="n">
-        <v>0.02241537267229051</v>
+        <v>0.03816901050718976</v>
       </c>
       <c r="E32" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.1071194811008229</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0.4741805467930643</v>
+        <v>0.77457885796807</v>
       </c>
       <c r="H32" t="n">
-        <v>-1.351307111227777</v>
+        <v>-1.19056230018322</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -1444,29 +1444,29 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-3)Gal</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1.943638386533586</v>
+        <v>0.2089220308636302</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.4549889041294808</v>
+        <v>-0.3930431878933027</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02237212616009071</v>
+        <v>0.04454391116254911</v>
       </c>
       <c r="E33" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.1183370757174649</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.4107615392457032</v>
+        <v>0.8324523277404274</v>
       </c>
       <c r="H33" t="n">
-        <v>-1.357098367751221</v>
+        <v>-1.106422179115075</v>
       </c>
       <c r="I33" t="n">
         <v>1</v>
@@ -1475,29 +1475,29 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_GalNAc(a1-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.5663672770895625</v>
+        <v>0.2001838225020558</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.4336665085774416</v>
+        <v>-0.5697466845819368</v>
       </c>
       <c r="D34" t="n">
-        <v>0.02154509246683057</v>
+        <v>0.04488647699627978</v>
       </c>
       <c r="E34" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.1183370757174649</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H34" t="n">
-        <v>-1.348344189917134</v>
+        <v>-1.121326214225566</v>
       </c>
       <c r="I34" t="n">
         <v>1</v>
@@ -1506,218 +1506,218 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)</t>
+          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1.88351148182623</v>
+        <v>0.5668520658313799</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.495411924784932</v>
+        <v>-0.4169334849834478</v>
       </c>
       <c r="D35" t="n">
-        <v>0.02434824249602397</v>
+        <v>0.05548628182690844</v>
       </c>
       <c r="E35" t="n">
-        <v>0.06634537794412967</v>
+        <v>0.1304677437551631</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0.8790855506262389</v>
+        <v>0.3186039900239953</v>
       </c>
       <c r="H35" t="n">
-        <v>-1.309160555999656</v>
+        <v>-1.093111405560048</v>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)GalNAc</t>
+          <t>Terminal_Fuc(a1-2)Gal(b1-3)GlcNAc</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.9086031766297306</v>
+        <v>0.2248309486646301</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.4273779260483019</v>
+        <v>-0.5908208008589657</v>
       </c>
       <c r="D36" t="n">
-        <v>0.03068283555453801</v>
+        <v>0.05504805087996232</v>
       </c>
       <c r="E36" t="n">
-        <v>0.07539211021972199</v>
+        <v>0.1304677437551631</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0.650792087649344</v>
+        <v>0.3928729275498804</v>
       </c>
       <c r="H36" t="n">
-        <v>-1.251872187481693</v>
+        <v>-1.058359467185971</v>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-4)Gal(b1-3)GalNAc</t>
+          <t>Terminal_GalNAc(a1-3)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.5500076852824186</v>
+        <v>0.05462725107780319</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.426054708589048</v>
+        <v>-0.6541000342430898</v>
       </c>
       <c r="D37" t="n">
-        <v>0.04256964275403916</v>
+        <v>0.05294311538350196</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1016941465790935</v>
+        <v>0.1304677437551631</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.2691002775158839</v>
       </c>
       <c r="H37" t="n">
-        <v>-1.165155564595873</v>
+        <v>-1.077608040383313</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-6)GlcNAc</t>
+          <t>Terminal_Gal(?1-?)GlcNAc(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.06857093566243377</v>
+        <v>0.9069961590286142</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.5635985082721763</v>
+        <v>-0.4007504070842574</v>
       </c>
       <c r="D38" t="n">
-        <v>0.05089539369539559</v>
+        <v>0.05421216744816539</v>
       </c>
       <c r="E38" t="n">
-        <v>0.1182974015622708</v>
+        <v>0.1304677437551631</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>0.3004829382090763</v>
+        <v>0.5508458305351739</v>
       </c>
       <c r="H38" t="n">
-        <v>-1.136109785066677</v>
+        <v>-1.093089156097396</v>
       </c>
       <c r="I38" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Terminal_GalOS(b1-3)GalNAc</t>
+          <t>Terminal_Fuc(a1-?)[HexNAc(?1-?)]GalNAc</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.003325937320055514</v>
+        <v>0.007537570096665078</v>
       </c>
       <c r="C39" t="n">
-        <v>1.213004065431961</v>
+        <v>-0.3837481683902295</v>
       </c>
       <c r="D39" t="n">
-        <v>0.06313966978057005</v>
+        <v>0.0615616249889469</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1428950421349743</v>
+        <v>0.1337361087602207</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0.5909631192162319</v>
+        <v>0.5389670244540066</v>
       </c>
       <c r="H39" t="n">
-        <v>1.056348400186054</v>
+        <v>-1.022376155187335</v>
       </c>
       <c r="I39" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(a1-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_GalOS(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.2000754041637939</v>
+        <v>0.003331872001774811</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.5328079975357949</v>
+        <v>1.214716530956003</v>
       </c>
       <c r="D40" t="n">
-        <v>0.06658641718028145</v>
+        <v>0.06177035279564293</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1468315866026719</v>
+        <v>0.1337361087602207</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>0.3004829382090763</v>
+        <v>0.5240530363668825</v>
       </c>
       <c r="H40" t="n">
-        <v>-1.012760855816875</v>
+        <v>1.062681313781922</v>
       </c>
       <c r="I40" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)Gal(b1-?)</t>
+          <t>Terminal_Gal(b1-3)[GlcNAcOS(b1-6)]GalNAc</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1.080039936374665</v>
+        <v>0.02119887516353442</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.3973393250267909</v>
+        <v>0.7504509352502795</v>
       </c>
       <c r="D41" t="n">
-        <v>0.06939958061698058</v>
+        <v>0.06469500142018041</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1487039769869901</v>
+        <v>0.1337361087602207</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.3309472900020025</v>
+        <v>0.5389670244540066</v>
       </c>
       <c r="H41" t="n">
-        <v>-1.01599823288058</v>
+        <v>1.021670982147337</v>
       </c>
       <c r="I41" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="42">
@@ -1727,28 +1727,28 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.02086112606070329</v>
+        <v>0.02089145170727644</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9659661148572384</v>
+        <v>0.9765817982750592</v>
       </c>
       <c r="D42" t="n">
-        <v>0.07089375647054177</v>
+        <v>0.06688777641584392</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1487039769869901</v>
+        <v>0.1337361087602207</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0.8426582200271998</v>
+        <v>0.7440563430518369</v>
       </c>
       <c r="H42" t="n">
-        <v>0.981001076693497</v>
+        <v>0.9978842808884667</v>
       </c>
       <c r="I42" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="43">
@@ -1758,28 +1758,28 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.8307898255762435</v>
+        <v>0.8315613173496219</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.393782899694795</v>
+        <v>-0.3930425934382065</v>
       </c>
       <c r="D43" t="n">
-        <v>0.07405282116339271</v>
+        <v>0.06700061303119875</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1516319671440898</v>
+        <v>0.1337361087602207</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.3000955164596797</v>
       </c>
       <c r="H43" t="n">
-        <v>-0.9664968371149995</v>
+        <v>-0.9968435008182748</v>
       </c>
       <c r="I43" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="44">
@@ -1789,214 +1789,214 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.871945675086353</v>
+        <v>0.8727596176779617</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.3756444744425496</v>
+        <v>-0.3775790466798146</v>
       </c>
       <c r="D44" t="n">
-        <v>0.07651662109454085</v>
+        <v>0.06760614811094939</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1530332421890817</v>
+        <v>0.1337361087602207</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.3153654155944906</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.9570845053291707</v>
+        <v>-0.9937259893807713</v>
       </c>
       <c r="I44" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)[GlcNAcOS(b1-6)]GalNAc</t>
+          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.021167265006762</v>
+        <v>0.3134182635386787</v>
       </c>
       <c r="C45" t="n">
-        <v>0.6797057942178205</v>
+        <v>-0.4631000058436991</v>
       </c>
       <c r="D45" t="n">
-        <v>0.07899013347778545</v>
+        <v>0.0676366527063185</v>
       </c>
       <c r="E45" t="n">
-        <v>0.1543898063429443</v>
+        <v>0.1337361087602207</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0.6272132120972961</v>
+        <v>0.5036187079846909</v>
       </c>
       <c r="H45" t="n">
-        <v>0.9614588920682773</v>
+        <v>-1.003028217335425</v>
       </c>
       <c r="I45" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-2)Gal(b1-3)GlcNAc</t>
+          <t>Terminal_GalNAc(a1-3)Gal(b1-3)GlcNAc</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.2246855686535541</v>
+        <v>0.1455565714242526</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.5355298680731959</v>
+        <v>-0.532413487925731</v>
       </c>
       <c r="D46" t="n">
-        <v>0.08850399190275127</v>
+        <v>0.07823914414572769</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1591614862506498</v>
+        <v>0.1512623453484069</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.411287053514931</v>
+        <v>0.5240530363668825</v>
       </c>
       <c r="H46" t="n">
-        <v>-0.9255665704721792</v>
+        <v>-0.9537809496043922</v>
       </c>
       <c r="I46" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)[HexNAc(?1-?)]GalNAc</t>
+          <t>Terminal_GalNAc(b1-4)GlcNAc(b1-6)</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.00753128450833863</v>
+        <v>0.7768986948710058</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.3495989159754154</v>
+        <v>-0.367630607812627</v>
       </c>
       <c r="D47" t="n">
-        <v>0.08883431790733944</v>
+        <v>0.08309081987193251</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1591614862506498</v>
+        <v>0.157072186936512</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0.5407217384221569</v>
+        <v>0.3186039900239953</v>
       </c>
       <c r="H47" t="n">
-        <v>-0.9174221576004481</v>
+        <v>-0.9370329000884855</v>
       </c>
       <c r="I47" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)</t>
+          <t>Terminal_Fuc(a1-3)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1.451756152271324</v>
+        <v>0.2649792934697341</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.3628480387245361</v>
+        <v>-0.4074211404970089</v>
       </c>
       <c r="D48" t="n">
-        <v>0.08547971537863462</v>
+        <v>0.08485508949443754</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1591614862506498</v>
+        <v>0.157072186936512</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0.3892258307000309</v>
+        <v>0.3153654155944906</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.9554039677724822</v>
+        <v>-0.9519656962333851</v>
       </c>
       <c r="I48" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-3)Gal</t>
+          <t>Terminal_Fuc(a1-3)GlcNAc(b1-3)Gal</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.2087536238077383</v>
+        <v>0.2587556410600626</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.3564887076652745</v>
+        <v>-0.4061677747525381</v>
       </c>
       <c r="D49" t="n">
-        <v>0.0879251818681361</v>
+        <v>0.08974877334385417</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1591614862506498</v>
+        <v>0.1626696516857357</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0.650792087649344</v>
+        <v>0.3186039900239953</v>
       </c>
       <c r="H49" t="n">
-        <v>-0.917310685823417</v>
+        <v>-0.9350873694343793</v>
       </c>
       <c r="I49" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(b1-4)GlcNAc(b1-6)</t>
+          <t>Terminal_HexNAc(?1-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.7762048001288639</v>
+        <v>1.081018680968725</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.3673935087007214</v>
+        <v>-0.3983901191280443</v>
       </c>
       <c r="D50" t="n">
-        <v>0.09159264472497379</v>
+        <v>0.09639821811914365</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1607544376805663</v>
+        <v>0.1711560199258265</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.9070081643590145</v>
+        <v>-0.9233836905952406</v>
       </c>
       <c r="I50" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="51">
@@ -2006,28 +2006,28 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.4673908194029502</v>
+        <v>0.4566334359640706</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.5396951167046438</v>
+        <v>-0.6542036721699964</v>
       </c>
       <c r="D51" t="n">
-        <v>0.1117134144946288</v>
+        <v>0.1038330598453232</v>
       </c>
       <c r="E51" t="n">
-        <v>0.1921470729307616</v>
+        <v>0.1806695241308624</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>0.2088724351931368</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H51" t="n">
-        <v>-0.8768281108038753</v>
+        <v>-0.9088029805725109</v>
       </c>
       <c r="I51" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="52">
@@ -2037,1299 +2037,1299 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.07956583574804765</v>
+        <v>0.07965168048836967</v>
       </c>
       <c r="C52" t="n">
-        <v>0.532167273565447</v>
+        <v>0.571543124396533</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1341393289744143</v>
+        <v>0.1126930029392365</v>
       </c>
       <c r="E52" t="n">
-        <v>0.2246276921596352</v>
+        <v>0.1922410050139917</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.3326234768490384</v>
       </c>
       <c r="H52" t="n">
-        <v>0.831828568094708</v>
+        <v>0.8889284127408967</v>
       </c>
       <c r="I52" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)HexNAc(?1-?)GlcNAc</t>
+          <t>Terminal_HexNAc(?1-?)</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.1045166047991759</v>
+        <v>1.453089445392603</v>
       </c>
       <c r="C53" t="n">
-        <v>-1.513941122114815</v>
+        <v>-0.3490503987803129</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1358213952593143</v>
+        <v>0.1301993632601594</v>
       </c>
       <c r="E53" t="n">
-        <v>0.2246276921596352</v>
+        <v>0.217833550069882</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>0.4071448117998211</v>
+        <v>0.2639442526448085</v>
       </c>
       <c r="H53" t="n">
-        <v>-0.8412379931043275</v>
+        <v>-0.830445597114866</v>
       </c>
       <c r="I53" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-3)Man(b1-4)GlcNAc</t>
+          <t>Terminal_Neu5Ac(a2-?)HexNAc(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.07498228082596464</v>
+        <v>0.1051887297837054</v>
       </c>
       <c r="C54" t="n">
-        <v>0.5374228199711302</v>
+        <v>-1.499784011705625</v>
       </c>
       <c r="D54" t="n">
-        <v>0.1405745221410369</v>
+        <v>0.1361258943648855</v>
       </c>
       <c r="E54" t="n">
-        <v>0.22810205479489</v>
+        <v>0.2234519398065101</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
       </c>
       <c r="G54" t="n">
-        <v>0.2115722175417238</v>
+        <v>0.401701710662534</v>
       </c>
       <c r="H54" t="n">
-        <v>0.8126525686350591</v>
+        <v>-0.8405160751094073</v>
       </c>
       <c r="I54" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(a1-3)Gal(b1-3)GlcNAc</t>
+          <t>Terminal_HexNAc(b1-?)GlcNAc(b1-?)</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1454814410118951</v>
+        <v>0.4070667730799701</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.4595930005664774</v>
+        <v>-0.2878280733160157</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1479082673463627</v>
+        <v>0.1503849206760482</v>
       </c>
       <c r="E55" t="n">
-        <v>0.235557610959022</v>
+        <v>0.2417330358558153</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0.5164195481440036</v>
+        <v>0.6375714441199014</v>
       </c>
       <c r="H55" t="n">
-        <v>-0.7702824424520928</v>
+        <v>-0.7621823897498781</v>
       </c>
       <c r="I55" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GalNAc</t>
+          <t>Terminal_Man(a1-3)Man(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.5136726592851022</v>
+        <v>0.07508733127114374</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.366892572353092</v>
+        <v>0.533269185835259</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1591747972141568</v>
+        <v>0.1528197353111476</v>
       </c>
       <c r="E56" t="n">
-        <v>0.2488915010984998</v>
+        <v>0.2417330358558153</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>0.2193683459696711</v>
+        <v>0.2591904674550313</v>
       </c>
       <c r="H56" t="n">
-        <v>-0.7622635109207853</v>
+        <v>0.7859529678709265</v>
       </c>
       <c r="I56" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-?)Gal(b1-?)</t>
+          <t>Terminal_HexNAc(?1-?)Gal(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1.1494537556622</v>
+        <v>0.5141666151373455</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.3328509850158436</v>
+        <v>-0.3846968928715881</v>
       </c>
       <c r="D57" t="n">
-        <v>0.1707378874256557</v>
+        <v>0.1576507408085837</v>
       </c>
       <c r="E57" t="n">
-        <v>0.2622046128322569</v>
+        <v>0.2449216866133353</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>0.3436622619306631</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.7410454500750314</v>
+        <v>-0.7672514320241098</v>
       </c>
       <c r="I57" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)[Neu5Ac(a2-6)]GalNAc</t>
+          <t>Terminal_Neu5Gc(a2-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.03279259865609406</v>
+        <v>0.1818801007831059</v>
       </c>
       <c r="C58" t="n">
-        <v>0.4371362466054043</v>
+        <v>0.6209718954352987</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1774334417788561</v>
+        <v>0.1705014231153958</v>
       </c>
       <c r="E58" t="n">
-        <v>0.2677065963680987</v>
+        <v>0.2602390142287621</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H58" t="n">
-        <v>0.7382305914416339</v>
+        <v>0.7439700583099589</v>
       </c>
       <c r="I58" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(b1-?)GlcNAc(b1-?)</t>
+          <t>Terminal_Neu5Gc(a2-?)</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.4067298279313263</v>
+        <v>0.3808186006393586</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.2811831783377783</v>
+        <v>0.5877432080377565</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1811910560716785</v>
+        <v>0.1922791155307467</v>
       </c>
       <c r="E59" t="n">
-        <v>0.2686626003821441</v>
+        <v>0.2857955306656472</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>0.9913355832782565</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H59" t="n">
-        <v>-0.7036417472849748</v>
+        <v>0.7060748549150528</v>
       </c>
       <c r="I59" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Gc(a2-?)</t>
+          <t>Terminal_GlcNAc(a1-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.3800921015120104</v>
+        <v>1.150640079191502</v>
       </c>
       <c r="C60" t="n">
-        <v>0.5776855657132569</v>
+        <v>-0.3331189291486183</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1899671779967162</v>
+        <v>0.1938153598767033</v>
       </c>
       <c r="E60" t="n">
-        <v>0.2769013103002981</v>
+        <v>0.2857955306656472</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
       </c>
       <c r="G60" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.3000955164596797</v>
       </c>
       <c r="H60" t="n">
-        <v>0.7093869519327333</v>
+        <v>-0.7011128112802297</v>
       </c>
       <c r="I60" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)Gal</t>
+          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)GalNAc</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.5447990415545709</v>
+        <v>0.06088627488828755</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.3265661623706979</v>
+        <v>-0.9265702263954319</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1965690294730174</v>
+        <v>0.2072353366107917</v>
       </c>
       <c r="E61" t="n">
-        <v>0.278507015002315</v>
+        <v>0.2955651522153914</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>0.3309472900020025</v>
+        <v>0.7308290891056934</v>
       </c>
       <c r="H61" t="n">
-        <v>-0.6880860061792919</v>
+        <v>-0.6627841373449477</v>
       </c>
       <c r="I61" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Gc(a2-6)GalNAc</t>
+          <t>Terminal_Man(a1-3)</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.1255451633043408</v>
+        <v>0.3617419494560898</v>
       </c>
       <c r="C62" t="n">
-        <v>0.5858744164981806</v>
+        <v>0.4392870580824031</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2004476224067075</v>
+        <v>0.2071919647750157</v>
       </c>
       <c r="E62" t="n">
-        <v>0.278507015002315</v>
+        <v>0.2955651522153914</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H62" t="n">
-        <v>0.6896729730219375</v>
+        <v>0.6799490125466408</v>
       </c>
       <c r="I62" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Gc(a2-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_Gal(b1-3)[Neu5Ac(a2-6)]GalNAc</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.1814438065409228</v>
+        <v>0.03283563925235573</v>
       </c>
       <c r="C63" t="n">
-        <v>0.5630223529149083</v>
+        <v>0.4364799336818333</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2007841270946922</v>
+        <v>0.2190757236314962</v>
       </c>
       <c r="E63" t="n">
-        <v>0.278507015002315</v>
+        <v>0.3074127089667769</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H63" t="n">
-        <v>0.6885986327523128</v>
+        <v>0.6673628632136531</v>
       </c>
       <c r="I63" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)GlcNAc(b1-?)GalNAc</t>
+          <t>Terminal_Neu5Gc(a2-3)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.06080412442921231</v>
+        <v>0.07321144816873229</v>
       </c>
       <c r="C64" t="n">
-        <v>-0.9154860816246442</v>
+        <v>0.5936580998760664</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2093691937632847</v>
+        <v>0.2233168788172933</v>
       </c>
       <c r="E64" t="n">
-        <v>0.2858055660895633</v>
+        <v>0.3083899755095955</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0.7336546162927878</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H64" t="n">
-        <v>-0.6593423023047161</v>
+        <v>0.6532562052461314</v>
       </c>
       <c r="I64" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Gc(a2-3)Gal(b1-3)GalNAc</t>
+          <t>Terminal_Man(a1-3)[Man(a1-6)]Man</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.07310313166674691</v>
+        <v>0.2866546181849461</v>
       </c>
       <c r="C65" t="n">
-        <v>0.5833255503136091</v>
+        <v>0.4117029581268743</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2268446123675446</v>
+        <v>0.2327794770186137</v>
       </c>
       <c r="E65" t="n">
-        <v>0.2934118913652114</v>
+        <v>0.3148935548286157</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H65" t="n">
-        <v>0.6476602220846895</v>
+        <v>0.639278298578821</v>
       </c>
       <c r="I65" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)</t>
+          <t>Terminal_Neu5Gc(a2-6)GalNAc</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.4007544592282248</v>
+        <v>0.1257270516875204</v>
       </c>
       <c r="C66" t="n">
-        <v>0.3955812595501755</v>
+        <v>0.5410024683136678</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2297700189614791</v>
+        <v>0.2376834528436524</v>
       </c>
       <c r="E66" t="n">
-        <v>0.2934118913652114</v>
+        <v>0.3148935548286157</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>0.3004829382090763</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H66" t="n">
-        <v>0.6329006249704242</v>
+        <v>0.6317367534388705</v>
       </c>
       <c r="I66" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)GalNAc</t>
+          <t>Terminal_Man(a1-?)</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.01012088087557708</v>
+        <v>1.172151102861013</v>
       </c>
       <c r="C67" t="n">
-        <v>-0.3368607183832317</v>
+        <v>0.3891071122769443</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2310173341956054</v>
+        <v>0.2388847657320533</v>
       </c>
       <c r="E67" t="n">
-        <v>0.2934118913652114</v>
+        <v>0.3148935548286157</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>0.7315913230211807</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H67" t="n">
-        <v>-0.6269036320381929</v>
+        <v>0.629315897826638</v>
       </c>
       <c r="I67" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)</t>
+          <t>Terminal_Man(a1-?)Man(a1-?)Man</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.4079669268342188</v>
+        <v>1.097063771589869</v>
       </c>
       <c r="C68" t="n">
-        <v>-0.3020766557435368</v>
+        <v>0.3780969699876273</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2327813811619523</v>
+        <v>0.2503461991579451</v>
       </c>
       <c r="E68" t="n">
-        <v>0.2934118913652114</v>
+        <v>0.3250764078618093</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>0.5407217384221569</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H68" t="n">
-        <v>-0.6262960478977792</v>
+        <v>0.6127551423914802</v>
       </c>
       <c r="I68" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-3)</t>
+          <t>Terminal_Man(a1-2)Man(a1-3)Man</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.3612482271641541</v>
+        <v>0.2334340087938186</v>
       </c>
       <c r="C69" t="n">
-        <v>0.4202857725146414</v>
+        <v>0.3813628312194499</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2342912864599442</v>
+        <v>0.255582842638709</v>
       </c>
       <c r="E69" t="n">
-        <v>0.2934118913652114</v>
+        <v>0.3269956957289364</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H69" t="n">
-        <v>0.6381752304498312</v>
+        <v>0.6059936145759539</v>
       </c>
       <c r="I69" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)Gal</t>
+          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.3978460459586418</v>
+        <v>0.4014623158676776</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.3006841092600725</v>
+        <v>0.3730646266922792</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2354118663279021</v>
+        <v>0.2598716206022276</v>
       </c>
       <c r="E70" t="n">
-        <v>0.2934118913652114</v>
+        <v>0.3276642172810695</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>0.5439964030143809</v>
+        <v>0.2691002775158839</v>
       </c>
       <c r="H70" t="n">
-        <v>-0.6225316169692504</v>
+        <v>0.5917326247146907</v>
       </c>
       <c r="I70" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)</t>
+          <t>Terminal_Gal(b1-?)GlcNAc(b1-?)Gal</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.4528692101368805</v>
+        <v>0.5458567498229276</v>
       </c>
       <c r="C71" t="n">
-        <v>0.3500368951589308</v>
+        <v>-0.2696566113638252</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2485903006410994</v>
+        <v>0.2687456078795817</v>
       </c>
       <c r="E71" t="n">
-        <v>0.3054109407876364</v>
+        <v>0.334012398364623</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>0.2913356450471932</v>
+        <v>0.2800068618095923</v>
       </c>
       <c r="H71" t="n">
-        <v>0.6089345235318347</v>
+        <v>-0.582509004165304</v>
       </c>
       <c r="I71" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Terminal_Gal(?1-?)Gal(?1-?)GlcNAc</t>
+          <t>Terminal_Man(a1-2)Man(a1-6)Man</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.02971731702513389</v>
+        <v>0.1040624161020581</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.2307087247528217</v>
+        <v>0.325878689478116</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2562447101238386</v>
+        <v>0.2734381395646348</v>
       </c>
       <c r="E72" t="n">
-        <v>0.3103809164880298</v>
+        <v>0.3350580020017355</v>
       </c>
       <c r="F72" t="b">
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>0.3004829382090763</v>
+        <v>0.2691002775158839</v>
       </c>
       <c r="H72" t="n">
-        <v>-0.5962788285718283</v>
+        <v>0.578373654466562</v>
       </c>
       <c r="I72" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-3)[Man(a1-6)]Man</t>
+          <t>Terminal_Man(a1-2)</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.2862659463381895</v>
+        <v>0.5237545352199768</v>
       </c>
       <c r="C73" t="n">
-        <v>0.3879381423499519</v>
+        <v>0.3408145727223029</v>
       </c>
       <c r="D73" t="n">
-        <v>0.2715619843777362</v>
+        <v>0.2775773942733792</v>
       </c>
       <c r="E73" t="n">
-        <v>0.324365703562296</v>
+        <v>0.3354060180803332</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2639442526448085</v>
       </c>
       <c r="H73" t="n">
-        <v>0.5858445792933451</v>
+        <v>0.5749028200225345</v>
       </c>
       <c r="I73" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-?)</t>
+          <t>Terminal_Neu5Ac(a2-3)</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>1.170601669326222</v>
+        <v>0.4535777116533252</v>
       </c>
       <c r="C74" t="n">
-        <v>0.3668172293676326</v>
+        <v>0.3249936813330367</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2882302513859978</v>
+        <v>0.288408749667054</v>
       </c>
       <c r="E74" t="n">
-        <v>0.3395589262903536</v>
+        <v>0.3437200167264891</v>
       </c>
       <c r="F74" t="b">
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2639442526448085</v>
       </c>
       <c r="H74" t="n">
-        <v>0.5641608762940972</v>
+        <v>0.5579462941910515</v>
       </c>
       <c r="I74" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-6)GalNAc</t>
+          <t>Terminal_Gal(a1-?)Gal(b1-?)</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.17776712589431</v>
+        <v>0.1684091096848624</v>
       </c>
       <c r="C75" t="n">
-        <v>0.3661212022494378</v>
+        <v>0.2165983650243544</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2949057581368515</v>
+        <v>0.2931750138730059</v>
       </c>
       <c r="E75" t="n">
-        <v>0.342728313510395</v>
+        <v>0.3446787325263717</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.8129643318725018</v>
       </c>
       <c r="H75" t="n">
-        <v>0.5555058138646919</v>
+        <v>0.5461140215404973</v>
       </c>
       <c r="I75" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-?)Man(a1-?)Man</t>
+          <t>Terminal_GalNAc(b1-?)[Fuc(a1-?)]GlcNAc</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1.095619388500257</v>
+        <v>0.05466262247861608</v>
       </c>
       <c r="C76" t="n">
-        <v>0.3545177568835252</v>
+        <v>-1.188775742842408</v>
       </c>
       <c r="D76" t="n">
-        <v>0.3045376667118556</v>
+        <v>0.3064563374577747</v>
       </c>
       <c r="E76" t="n">
-        <v>0.348313525528714</v>
+        <v>0.3554893514510187</v>
       </c>
       <c r="F76" t="b">
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.7110222513655526</v>
       </c>
       <c r="H76" t="n">
-        <v>0.5441022794860186</v>
+        <v>-0.5321834965271689</v>
       </c>
       <c r="I76" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Terminal_GalNAc(b1-?)[Fuc(a1-?)]GlcNAc</t>
+          <t>Terminal_Neu5Ac(a2-6)GalNAc</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.05458502544737925</v>
+        <v>0.1780055171358561</v>
       </c>
       <c r="C77" t="n">
-        <v>-1.176687184979679</v>
+        <v>0.3607841990699063</v>
       </c>
       <c r="D77" t="n">
-        <v>0.3085506750483685</v>
+        <v>0.31458114764196</v>
       </c>
       <c r="E77" t="n">
-        <v>0.348313525528714</v>
+        <v>0.355899868141521</v>
       </c>
       <c r="F77" t="b">
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>0.7315913230211807</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H77" t="n">
-        <v>-0.5297013000992509</v>
+        <v>0.5324718184909328</v>
       </c>
       <c r="I77" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-4)</t>
+          <t>Terminal_Man(?1-?)</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2.079365864040508</v>
+        <v>0.2380585044199082</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.2670329269578975</v>
+        <v>0.3391297522976413</v>
       </c>
       <c r="D78" t="n">
-        <v>0.3118621100664067</v>
+        <v>0.3149918373206565</v>
       </c>
       <c r="E78" t="n">
-        <v>0.348313525528714</v>
+        <v>0.355899868141521</v>
       </c>
       <c r="F78" t="b">
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>0.3004829382090763</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H78" t="n">
-        <v>-0.5310089657745694</v>
+        <v>0.5298316381242021</v>
       </c>
       <c r="I78" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-2)Man(a1-3)Man</t>
+          <t>Terminal_Gal(?1-?)Gal(?1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.2331269147934129</v>
+        <v>0.02974055102503284</v>
       </c>
       <c r="C79" t="n">
-        <v>0.3479804025204833</v>
+        <v>-0.1860200895809908</v>
       </c>
       <c r="D79" t="n">
-        <v>0.324495295202691</v>
+        <v>0.3216898092927002</v>
       </c>
       <c r="E79" t="n">
-        <v>0.3535333005396828</v>
+        <v>0.3569345753021032</v>
       </c>
       <c r="F79" t="b">
         <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.5508458305351739</v>
       </c>
       <c r="H79" t="n">
-        <v>0.5212251026031011</v>
+        <v>-0.5156908260325505</v>
       </c>
       <c r="I79" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_Man(a1-2)Man(a1-2)Man</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.1025820326840233</v>
+        <v>0.1862581103241</v>
       </c>
       <c r="C80" t="n">
-        <v>0.5392636557773792</v>
+        <v>0.2953739580039683</v>
       </c>
       <c r="D80" t="n">
-        <v>0.3256876583465538</v>
+        <v>0.324113005159381</v>
       </c>
       <c r="E80" t="n">
-        <v>0.3535333005396828</v>
+        <v>0.3569345753021032</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0.7315913230211807</v>
+        <v>0.2639442526448085</v>
       </c>
       <c r="H80" t="n">
-        <v>0.509301412076689</v>
+        <v>0.5176678480059963</v>
       </c>
       <c r="I80" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Terminal_Gal(a1-?)Gal(b1-?)</t>
+          <t>Terminal_Neu5Ac(a2-3)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.1681985713823398</v>
+        <v>0.1026958119087756</v>
       </c>
       <c r="C81" t="n">
-        <v>0.1885747785532998</v>
+        <v>0.5402294332822027</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3288681865485421</v>
+        <v>0.3328503555856617</v>
       </c>
       <c r="E81" t="n">
-        <v>0.3535333005396828</v>
+        <v>0.3619747616994071</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>0.7315913230211807</v>
+        <v>0.77457885796807</v>
       </c>
       <c r="H81" t="n">
-        <v>0.5060982064423019</v>
+        <v>0.5015347216452758</v>
       </c>
       <c r="I81" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-6)GalNAc</t>
+          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.1979762041235879</v>
+        <v>0.01013104939887684</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.2085855159806718</v>
+        <v>-0.2872420599835883</v>
       </c>
       <c r="D82" t="n">
-        <v>0.3496990447712718</v>
+        <v>0.3492520002504018</v>
       </c>
       <c r="E82" t="n">
-        <v>0.3614112606812155</v>
+        <v>0.3751225187874687</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0.7099032064572747</v>
+        <v>0.3928729275498804</v>
       </c>
       <c r="H82" t="n">
-        <v>-0.4838043574641733</v>
+        <v>-0.4859304089615366</v>
       </c>
       <c r="I82" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-2)Man(a1-6)Man</t>
+          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.1039346101038845</v>
+        <v>0.2831678288362356</v>
       </c>
       <c r="C83" t="n">
-        <v>0.3086446275923926</v>
+        <v>0.3253852297392479</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3530063476421175</v>
+        <v>0.3944610221299358</v>
       </c>
       <c r="E83" t="n">
-        <v>0.3614112606812155</v>
+        <v>0.4093113633721923</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H83" t="n">
-        <v>0.4881083621517505</v>
+        <v>0.4469739382240178</v>
       </c>
       <c r="I83" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)</t>
+          <t>Terminal_GlcNAc(a1-4)</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.2826313167472345</v>
+        <v>2.081499748153279</v>
       </c>
       <c r="C84" t="n">
-        <v>0.3597414203349212</v>
+        <v>-0.2309010567582925</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3457980723895209</v>
+        <v>0.3951971784283236</v>
       </c>
       <c r="E84" t="n">
-        <v>0.3614112606812155</v>
+        <v>0.4093113633721923</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2691002775158839</v>
       </c>
       <c r="H84" t="n">
-        <v>0.4970627092249619</v>
+        <v>-0.4436682851824755</v>
       </c>
       <c r="I84" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-2)</t>
+          <t>Terminal_HexNAc(b1-4)GlcNAc(b1-6)GalNAc</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.523087495823878</v>
+        <v>0.19814474221634</v>
       </c>
       <c r="C85" t="n">
-        <v>0.3178555862535717</v>
+        <v>-0.1842436899412028</v>
       </c>
       <c r="D85" t="n">
-        <v>0.3493434543466507</v>
+        <v>0.3887157552496143</v>
       </c>
       <c r="E85" t="n">
-        <v>0.3614112606812155</v>
+        <v>0.4093113633721923</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.5240530363668825</v>
       </c>
       <c r="H85" t="n">
-        <v>0.4927479297954797</v>
+        <v>-0.4451169023682568</v>
       </c>
       <c r="I85" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Terminal_Man(?1-?)</t>
+          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)GlcNAc</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.2377461612236153</v>
+        <v>0.1182944870314419</v>
       </c>
       <c r="C86" t="n">
-        <v>0.3246525131241165</v>
+        <v>0.3344476826677947</v>
       </c>
       <c r="D86" t="n">
-        <v>0.3616009395111699</v>
+        <v>0.4145837198328608</v>
       </c>
       <c r="E86" t="n">
-        <v>0.3658550682113013</v>
+        <v>0.4243386308877516</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.5508458305351739</v>
       </c>
       <c r="H86" t="n">
-        <v>0.4795438243727845</v>
+        <v>0.4209096731414266</v>
       </c>
       <c r="I86" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)GalNAc</t>
+          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.3237871662573442</v>
+        <v>0.4088970062241618</v>
       </c>
       <c r="C87" t="n">
-        <v>0.3052390261193376</v>
+        <v>-0.2000475381484272</v>
       </c>
       <c r="D87" t="n">
-        <v>0.3782510180820927</v>
+        <v>0.4348744253946842</v>
       </c>
       <c r="E87" t="n">
-        <v>0.3782510180820927</v>
+        <v>0.4399311047597387</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.4881422173909434</v>
       </c>
       <c r="H87" t="n">
-        <v>0.4643580033651453</v>
+        <v>-0.403458943609927</v>
       </c>
       <c r="I87" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(a1-4)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_Gal(b1-4)GlcNAc(b1-3)Gal</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.599446070379781</v>
+        <v>0.398765956825285</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.25303242304226</v>
+        <v>-0.1975204351482329</v>
       </c>
       <c r="D88" t="n">
-        <v>0.3840480790741236</v>
+        <v>0.4403686858653848</v>
       </c>
       <c r="E88" t="n">
-        <v>0.3840480790741236</v>
+        <v>0.4403686858653848</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>0.3004829382090763</v>
+        <v>0.4995786509894896</v>
       </c>
       <c r="H88" t="n">
-        <v>-0.4555950634423882</v>
+        <v>-0.3984892301743765</v>
       </c>
       <c r="I88" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Terminal_Man(a1-2)Man(a1-2)Man</t>
+          <t>Terminal_Neu5Ac(a2-3)Gal(b1-3)GalNAc</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.1860259709265808</v>
+        <v>0.3243661291645755</v>
       </c>
       <c r="C89" t="n">
-        <v>0.2848113164916002</v>
+        <v>0.2656057013613009</v>
       </c>
       <c r="D89" t="n">
-        <v>0.3875792683591138</v>
+        <v>0.4478290924704103</v>
       </c>
       <c r="E89" t="n">
-        <v>0.3875792683591138</v>
+        <v>0.4478290924704103</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H89" t="n">
-        <v>0.4523663505129191</v>
+        <v>0.3977373482505133</v>
       </c>
       <c r="I89" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Terminal_Gal(a1-3)Gal(b1-4)GlcNAc</t>
+          <t>Terminal_Fuc(a1-?)[Gal(?1-?)]GlcNAc</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.08863273563429221</v>
+        <v>0.009462410643505659</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.1910381735439306</v>
+        <v>-0.8398024805072675</v>
       </c>
       <c r="D90" t="n">
-        <v>0.4193735941536998</v>
+        <v>0.4829186102306087</v>
       </c>
       <c r="E90" t="n">
-        <v>0.4193735941536998</v>
+        <v>0.4829186102306087</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>0.5611957331633769</v>
+        <v>0.8129643318725018</v>
       </c>
       <c r="H90" t="n">
-        <v>-0.4177400572007203</v>
+        <v>-0.3606037899090441</v>
       </c>
       <c r="I90" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)Gal(b1-?)GlcNAc</t>
+          <t>Terminal_GlcNAc(a1-4)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.1181231424809903</v>
+        <v>0.6000476859775833</v>
       </c>
       <c r="C91" t="n">
-        <v>0.3267612254709844</v>
+        <v>-0.2128759775878044</v>
       </c>
       <c r="D91" t="n">
-        <v>0.421237848422897</v>
+        <v>0.4905877382915402</v>
       </c>
       <c r="E91" t="n">
-        <v>0.421237848422897</v>
+        <v>0.4905877382915402</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>0.5909631192162319</v>
+        <v>0.2698604558267682</v>
       </c>
       <c r="H91" t="n">
-        <v>0.4148801251513961</v>
+        <v>-0.3586960140861148</v>
       </c>
       <c r="I91" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Terminal_Fuc(a1-?)[Gal(?1-?)]GlcNAc</t>
+          <t>Terminal_Gal(a1-3)Gal(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.009433881734720082</v>
+        <v>0.08875742919649275</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.8618790179232549</v>
+        <v>-0.1517850270052314</v>
       </c>
       <c r="D92" t="n">
-        <v>0.4738424166041377</v>
+        <v>0.5099827589717536</v>
       </c>
       <c r="E92" t="n">
-        <v>0.4738424166041377</v>
+        <v>0.5099827589717536</v>
       </c>
       <c r="F92" t="b">
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>0.8426582200271998</v>
+        <v>0.3186039900239953</v>
       </c>
       <c r="H92" t="n">
-        <v>-0.3682251537625333</v>
+        <v>-0.3398763151148962</v>
       </c>
       <c r="I92" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Terminal_GlcNAc(b1-4)Man(b1-4)GlcNAc</t>
+          <t>Terminal_Neu5Ac(a2-3)[GalNAc(b1-4)]Gal</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.01631263326284584</v>
+        <v>0.04119830032833986</v>
       </c>
       <c r="C93" t="n">
-        <v>0.7899040373568722</v>
+        <v>-0.08893889144579681</v>
       </c>
       <c r="D93" t="n">
-        <v>0.4904608834316769</v>
+        <v>0.7369333344403683</v>
       </c>
       <c r="E93" t="n">
-        <v>0.4904608834316769</v>
+        <v>0.7369333344403683</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>0.8513688280488774</v>
+        <v>0.2639442526448085</v>
       </c>
       <c r="H93" t="n">
-        <v>0.3543803639264408</v>
+        <v>-0.1722512100232603</v>
       </c>
       <c r="I93" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="94">
@@ -3339,121 +3339,121 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.9299121083783076</v>
+        <v>0.9308596689617763</v>
       </c>
       <c r="C94" t="n">
-        <v>-0.1816696445693484</v>
+        <v>-0.09884013593554286</v>
       </c>
       <c r="D94" t="n">
-        <v>0.5566723647854745</v>
+        <v>0.7487237651108944</v>
       </c>
       <c r="E94" t="n">
-        <v>0.5566723647854745</v>
+        <v>0.7487237651108944</v>
       </c>
       <c r="F94" t="b">
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>0.3090887083239104</v>
+        <v>0.3003363301440668</v>
       </c>
       <c r="H94" t="n">
-        <v>-0.3022936311012283</v>
+        <v>-0.1639033584654491</v>
       </c>
       <c r="I94" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Terminal_Gal(b1-3)[Neu5Gc(a2-6)]GalNAc</t>
+          <t>Terminal_GlcNAc(b1-4)Man(b1-4)GlcNAc</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.00367878742766069</v>
+        <v>0.01359456481336472</v>
       </c>
       <c r="C95" t="n">
-        <v>0.118648662231617</v>
+        <v>0.2648914474671691</v>
       </c>
       <c r="D95" t="n">
-        <v>0.7311840560010376</v>
+        <v>0.8112233405960931</v>
       </c>
       <c r="E95" t="n">
-        <v>0.7311840560010376</v>
+        <v>0.8112233405960931</v>
       </c>
       <c r="F95" t="b">
         <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.9888014237703878</v>
       </c>
       <c r="H95" t="n">
-        <v>0.177116506679248</v>
+        <v>0.1217612191322921</v>
       </c>
       <c r="I95" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-3)[GalNAc(b1-4)]Gal</t>
+          <t>Terminal_Neu5Ac(a2-?)</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.04115584951010972</v>
+        <v>1.182488299079649</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.03324335397585315</v>
+        <v>-0.01864755586353528</v>
       </c>
       <c r="D96" t="n">
-        <v>0.8965231743415183</v>
+        <v>0.8890377077690441</v>
       </c>
       <c r="E96" t="n">
-        <v>0.8965231743415183</v>
+        <v>0.8890377077690441</v>
       </c>
       <c r="F96" t="b">
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>0.2050991658004412</v>
+        <v>0.8129643318725018</v>
       </c>
       <c r="H96" t="n">
-        <v>-0.06649850912315906</v>
+        <v>-0.07104400565975642</v>
       </c>
       <c r="I96" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Terminal_Neu5Ac(a2-?)</t>
+          <t>Terminal_Gal(b1-3)[Neu5Gc(a2-6)]GalNAc</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>1.191584858834771</v>
+        <v>0.003683471420799203</v>
       </c>
       <c r="C97" t="n">
-        <v>0.004296310820306459</v>
+        <v>0.03032051753352061</v>
       </c>
       <c r="D97" t="n">
-        <v>0.9744408262043387</v>
+        <v>0.934813825689454</v>
       </c>
       <c r="E97" t="n">
-        <v>0.9744408262043387</v>
+        <v>0.934813825689454</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>0.8513688280488774</v>
+        <v>0.2305244964102945</v>
       </c>
       <c r="H97" t="n">
-        <v>0.01630833241295825</v>
+        <v>0.0420740904140233</v>
       </c>
       <c r="I97" t="n">
-        <v>0.9588931880689067</v>
+        <v>0.9521344926210376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>